<commit_message>
cambios de las notas
</commit_message>
<xml_diff>
--- a/OYM/_Documentos Comunes/BD_C32017.xlsx
+++ b/OYM/_Documentos Comunes/BD_C32017.xlsx
@@ -918,10 +918,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -930,14 +933,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -948,20 +951,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
@@ -969,16 +975,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1366,8 +1366,8 @@
   <dimension ref="A1:Z102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P32" sqref="P32"/>
+      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1398,19 +1398,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -1431,19 +1431,19 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
       <c r="N3" s="2"/>
       <c r="P3" t="s">
         <v>21</v>
@@ -1453,19 +1453,19 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
       <c r="N4" s="2"/>
       <c r="P4" t="s">
         <v>23</v>
@@ -1475,19 +1475,19 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
       <c r="N5" s="2"/>
       <c r="P5" t="s">
         <v>25</v>
@@ -1519,19 +1519,19 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
       <c r="N7" s="2"/>
       <c r="P7" t="s">
         <v>29</v>
@@ -1585,10 +1585,10 @@
       <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:26" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="25"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
         <v>2</v>
       </c>
@@ -1598,21 +1598,21 @@
       </c>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="25"/>
+      <c r="I10" s="23"/>
       <c r="J10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="25" t="s">
+      <c r="L10" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
       <c r="O10" s="2"/>
       <c r="P10" t="s">
         <v>8</v>
@@ -1649,35 +1649,35 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="26">
+      <c r="A11" s="28">
         <v>0</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="29"/>
+      <c r="C11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="28" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="13">
+      <c r="F11" s="13"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="14">
         <v>10</v>
       </c>
-      <c r="I11" s="14"/>
+      <c r="I11" s="15"/>
       <c r="J11" s="5">
         <v>20</v>
       </c>
       <c r="K11" s="5">
         <v>20</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="14">
         <f>IF((Y11-50)&gt;50,50,IF((Y11-50)&lt;0,0,(Y11-50)))</f>
         <v>50</v>
       </c>
-      <c r="M11" s="15"/>
-      <c r="N11" s="14"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="15"/>
       <c r="O11" s="2"/>
       <c r="P11">
         <v>20</v>
@@ -1715,52 +1715,52 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="18" t="s">
+      <c r="D12" s="20"/>
+      <c r="E12" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="14"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="15"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="15"/>
       <c r="O12" s="2"/>
       <c r="P12">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="18" t="s">
+      <c r="D13" s="20"/>
+      <c r="E13" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="14"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="15"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="15"/>
       <c r="O13" s="2"/>
       <c r="P13">
         <v>10</v>
@@ -1770,75 +1770,75 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="18" t="s">
+      <c r="D14" s="20"/>
+      <c r="E14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="14"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="15"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="15"/>
       <c r="O14" s="2"/>
     </row>
     <row r="15" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="18" t="s">
+      <c r="D15" s="20"/>
+      <c r="E15" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="14"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="15"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="15"/>
       <c r="O15" s="2"/>
       <c r="P15">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="18" t="s">
+      <c r="D16" s="20"/>
+      <c r="E16" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="14"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="15"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="15"/>
       <c r="O16" s="2"/>
       <c r="P16">
         <v>10</v>
@@ -1848,104 +1848,104 @@
       </c>
     </row>
     <row r="17" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18" t="s">
+      <c r="B17" s="26"/>
+      <c r="C17" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="18" t="s">
+      <c r="D17" s="20"/>
+      <c r="E17" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="14"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="15"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="15"/>
       <c r="O17" s="2"/>
       <c r="P17">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="26"/>
+      <c r="C18" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="18" t="s">
+      <c r="D18" s="20"/>
+      <c r="E18" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="20"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="14"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="15"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="15"/>
       <c r="O18" s="2"/>
       <c r="Q18">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18" t="s">
+      <c r="B19" s="26"/>
+      <c r="C19" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="18" t="s">
+      <c r="D19" s="20"/>
+      <c r="E19" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="20"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="14"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="15"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="15"/>
       <c r="O19" s="2"/>
       <c r="P19">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18" t="s">
+      <c r="B20" s="26"/>
+      <c r="C20" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="18" t="s">
+      <c r="D20" s="20"/>
+      <c r="E20" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="14"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="15"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="15"/>
       <c r="O20" s="2"/>
       <c r="P20">
         <v>11</v>
@@ -1955,52 +1955,52 @@
       </c>
     </row>
     <row r="21" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18" t="s">
+      <c r="B21" s="26"/>
+      <c r="C21" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="18" t="s">
+      <c r="D21" s="20"/>
+      <c r="E21" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="14"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="15"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="15"/>
       <c r="O21" s="2"/>
       <c r="P21">
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18" t="s">
+      <c r="B22" s="26"/>
+      <c r="C22" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="18" t="s">
+      <c r="D22" s="20"/>
+      <c r="E22" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="14"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="15"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="15"/>
       <c r="O22" s="2"/>
       <c r="P22">
         <v>8</v>
@@ -2010,49 +2010,49 @@
       </c>
     </row>
     <row r="23" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18" t="s">
+      <c r="B23" s="26"/>
+      <c r="C23" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="18" t="s">
+      <c r="D23" s="20"/>
+      <c r="E23" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="14"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="15"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="15"/>
       <c r="O23" s="2"/>
     </row>
     <row r="24" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18" t="s">
+      <c r="B24" s="26"/>
+      <c r="C24" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="18" t="s">
+      <c r="D24" s="20"/>
+      <c r="E24" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="14"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="15"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="15"/>
       <c r="O24" s="2"/>
       <c r="P24">
         <v>16</v>
@@ -2062,26 +2062,26 @@
       </c>
     </row>
     <row r="25" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18" t="s">
+      <c r="B25" s="26"/>
+      <c r="C25" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="18" t="s">
+      <c r="D25" s="20"/>
+      <c r="E25" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="14"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="15"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="15"/>
       <c r="O25" s="2"/>
       <c r="P25">
         <v>16</v>
@@ -2091,52 +2091,52 @@
       </c>
     </row>
     <row r="26" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18" t="s">
+      <c r="B26" s="26"/>
+      <c r="C26" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="18" t="s">
+      <c r="D26" s="20"/>
+      <c r="E26" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="14"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="15"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="15"/>
       <c r="O26" s="2"/>
       <c r="P26">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18" t="s">
+      <c r="B27" s="26"/>
+      <c r="C27" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="18" t="s">
+      <c r="D27" s="20"/>
+      <c r="E27" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="14"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="15"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="15"/>
       <c r="O27" s="2"/>
       <c r="P27">
         <v>12</v>
@@ -2146,26 +2146,26 @@
       </c>
     </row>
     <row r="28" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18" t="s">
+      <c r="B28" s="26"/>
+      <c r="C28" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="18" t="s">
+      <c r="D28" s="20"/>
+      <c r="E28" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="14"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="15"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="15"/>
       <c r="O28" s="2"/>
       <c r="P28">
         <v>11</v>
@@ -2175,26 +2175,26 @@
       </c>
     </row>
     <row r="29" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18" t="s">
+      <c r="B29" s="26"/>
+      <c r="C29" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="18" t="s">
+      <c r="D29" s="20"/>
+      <c r="E29" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="20"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="14"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="15"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="15"/>
       <c r="O29" s="2"/>
       <c r="P29">
         <v>13</v>
@@ -2204,26 +2204,26 @@
       </c>
     </row>
     <row r="30" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18" t="s">
+      <c r="B30" s="26"/>
+      <c r="C30" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="18" t="s">
+      <c r="D30" s="20"/>
+      <c r="E30" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="14"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="15"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="15"/>
       <c r="O30" s="2"/>
       <c r="P30">
         <v>11</v>
@@ -2233,101 +2233,101 @@
       </c>
     </row>
     <row r="31" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="18" t="s">
+      <c r="B31" s="26"/>
+      <c r="C31" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="18" t="s">
+      <c r="D31" s="20"/>
+      <c r="E31" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="F31" s="20"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="14"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="15"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="15"/>
       <c r="O31" s="2"/>
     </row>
     <row r="32" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="18" t="s">
+      <c r="B32" s="26"/>
+      <c r="C32" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="18" t="s">
+      <c r="D32" s="20"/>
+      <c r="E32" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="14"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="15"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="15"/>
       <c r="O32" s="2"/>
       <c r="P32">
         <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="18" t="s">
+      <c r="B33" s="26"/>
+      <c r="C33" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="18" t="s">
+      <c r="D33" s="20"/>
+      <c r="E33" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="F33" s="20"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="14"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="15"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="15"/>
       <c r="O33" s="2"/>
       <c r="Q33">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="18" t="s">
+      <c r="B34" s="26"/>
+      <c r="C34" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="18" t="s">
+      <c r="D34" s="20"/>
+      <c r="E34" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F34" s="20"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="14"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="15"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="15"/>
       <c r="O34" s="2"/>
       <c r="P34">
         <v>9</v>
@@ -2337,26 +2337,26 @@
       </c>
     </row>
     <row r="35" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="18" t="s">
+      <c r="B35" s="26"/>
+      <c r="C35" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="18" t="s">
+      <c r="D35" s="20"/>
+      <c r="E35" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="F35" s="20"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="14"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="15"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="15"/>
       <c r="O35" s="2"/>
       <c r="P35">
         <v>9</v>
@@ -2366,26 +2366,26 @@
       </c>
     </row>
     <row r="36" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="18" t="s">
+      <c r="B36" s="26"/>
+      <c r="C36" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="18" t="s">
+      <c r="D36" s="20"/>
+      <c r="E36" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="F36" s="20"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="14"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="15"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="15"/>
       <c r="O36" s="2"/>
       <c r="P36">
         <v>10</v>
@@ -2395,52 +2395,52 @@
       </c>
     </row>
     <row r="37" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="17"/>
-      <c r="C37" s="18" t="s">
+      <c r="B37" s="26"/>
+      <c r="C37" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="18" t="s">
+      <c r="D37" s="20"/>
+      <c r="E37" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="F37" s="20"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="14"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="15"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="22"/>
+      <c r="N37" s="15"/>
       <c r="O37" s="2"/>
       <c r="P37">
         <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="18" t="s">
+      <c r="B38" s="26"/>
+      <c r="C38" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="19"/>
-      <c r="E38" s="18" t="s">
+      <c r="D38" s="20"/>
+      <c r="E38" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F38" s="20"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="14"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="15"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="15"/>
       <c r="O38" s="2"/>
       <c r="P38">
         <v>8</v>
@@ -2450,26 +2450,26 @@
       </c>
     </row>
     <row r="39" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="17"/>
-      <c r="C39" s="18" t="s">
+      <c r="B39" s="26"/>
+      <c r="C39" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="18" t="s">
+      <c r="D39" s="20"/>
+      <c r="E39" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="F39" s="20"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="14"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="15"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="13"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="22"/>
+      <c r="N39" s="15"/>
       <c r="O39" s="2"/>
       <c r="P39">
         <v>8</v>
@@ -2479,26 +2479,26 @@
       </c>
     </row>
     <row r="40" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="18" t="s">
+      <c r="B40" s="26"/>
+      <c r="C40" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="19"/>
-      <c r="E40" s="18" t="s">
+      <c r="D40" s="20"/>
+      <c r="E40" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="F40" s="20"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="14"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="15"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
-      <c r="L40" s="13"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="22"/>
+      <c r="N40" s="15"/>
       <c r="O40" s="2"/>
       <c r="P40">
         <v>15</v>
@@ -2508,52 +2508,52 @@
       </c>
     </row>
     <row r="41" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="18" t="s">
+      <c r="B41" s="26"/>
+      <c r="C41" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="18" t="s">
+      <c r="D41" s="20"/>
+      <c r="E41" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F41" s="20"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="14"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="15"/>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="22"/>
+      <c r="N41" s="15"/>
       <c r="O41" s="2"/>
       <c r="Q41">
         <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="16" t="s">
+      <c r="A42" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="18" t="s">
+      <c r="B42" s="26"/>
+      <c r="C42" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="D42" s="19"/>
-      <c r="E42" s="18" t="s">
+      <c r="D42" s="20"/>
+      <c r="E42" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="F42" s="20"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="14"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="15"/>
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="22"/>
+      <c r="N42" s="15"/>
       <c r="O42" s="2"/>
       <c r="P42">
         <v>12</v>
@@ -2563,26 +2563,26 @@
       </c>
     </row>
     <row r="43" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="18" t="s">
+      <c r="B43" s="26"/>
+      <c r="C43" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="19"/>
-      <c r="E43" s="18" t="s">
+      <c r="D43" s="20"/>
+      <c r="E43" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="F43" s="20"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="14"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="15"/>
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
-      <c r="L43" s="13"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="22"/>
+      <c r="N43" s="15"/>
       <c r="O43" s="2"/>
       <c r="P43">
         <v>17</v>
@@ -2592,26 +2592,26 @@
       </c>
     </row>
     <row r="44" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="18" t="s">
+      <c r="B44" s="26"/>
+      <c r="C44" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="D44" s="19"/>
-      <c r="E44" s="18" t="s">
+      <c r="D44" s="20"/>
+      <c r="E44" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="F44" s="20"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="14"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="15"/>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
-      <c r="L44" s="13"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="22"/>
+      <c r="N44" s="15"/>
       <c r="O44" s="2"/>
       <c r="P44">
         <v>10</v>
@@ -2621,26 +2621,26 @@
       </c>
     </row>
     <row r="45" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="B45" s="17"/>
-      <c r="C45" s="18" t="s">
+      <c r="B45" s="26"/>
+      <c r="C45" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="18" t="s">
+      <c r="D45" s="20"/>
+      <c r="E45" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="F45" s="20"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="14"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="15"/>
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
-      <c r="L45" s="13"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="22"/>
+      <c r="N45" s="15"/>
       <c r="O45" s="2"/>
       <c r="P45">
         <v>19</v>
@@ -2650,26 +2650,26 @@
       </c>
     </row>
     <row r="46" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="B46" s="17"/>
-      <c r="C46" s="18" t="s">
+      <c r="B46" s="26"/>
+      <c r="C46" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="D46" s="19"/>
-      <c r="E46" s="18" t="s">
+      <c r="D46" s="20"/>
+      <c r="E46" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="F46" s="20"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="14"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="15"/>
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="14"/>
+      <c r="L46" s="14"/>
+      <c r="M46" s="22"/>
+      <c r="N46" s="15"/>
       <c r="O46" s="2"/>
       <c r="P46">
         <v>10</v>
@@ -2679,52 +2679,52 @@
       </c>
     </row>
     <row r="47" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="B47" s="17"/>
-      <c r="C47" s="18" t="s">
+      <c r="B47" s="26"/>
+      <c r="C47" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="D47" s="19"/>
-      <c r="E47" s="18" t="s">
+      <c r="D47" s="20"/>
+      <c r="E47" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="F47" s="20"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="14"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="15"/>
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
-      <c r="L47" s="13"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="22"/>
+      <c r="N47" s="15"/>
       <c r="O47" s="2"/>
       <c r="Q47">
         <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="16" t="s">
+      <c r="A48" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="18" t="s">
+      <c r="B48" s="26"/>
+      <c r="C48" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="D48" s="19"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="20"/>
+      <c r="E48" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="F48" s="20"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="14"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="15"/>
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
-      <c r="L48" s="13"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="22"/>
+      <c r="N48" s="15"/>
       <c r="O48" s="2"/>
       <c r="P48">
         <v>20</v>
@@ -2734,26 +2734,26 @@
       </c>
     </row>
     <row r="49" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="16" t="s">
+      <c r="A49" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="B49" s="17"/>
-      <c r="C49" s="18" t="s">
+      <c r="B49" s="26"/>
+      <c r="C49" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D49" s="19"/>
-      <c r="E49" s="18" t="s">
+      <c r="D49" s="20"/>
+      <c r="E49" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="F49" s="20"/>
-      <c r="G49" s="19"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="14"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="15"/>
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
-      <c r="L49" s="13"/>
-      <c r="M49" s="15"/>
-      <c r="N49" s="14"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="22"/>
+      <c r="N49" s="15"/>
       <c r="O49" s="2"/>
       <c r="P49">
         <v>17</v>
@@ -2763,26 +2763,26 @@
       </c>
     </row>
     <row r="50" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="16" t="s">
+      <c r="A50" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="B50" s="17"/>
-      <c r="C50" s="18" t="s">
+      <c r="B50" s="26"/>
+      <c r="C50" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="D50" s="19"/>
-      <c r="E50" s="18" t="s">
+      <c r="D50" s="20"/>
+      <c r="E50" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="F50" s="20"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="14"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="15"/>
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="15"/>
-      <c r="N50" s="14"/>
+      <c r="L50" s="14"/>
+      <c r="M50" s="22"/>
+      <c r="N50" s="15"/>
       <c r="O50" s="2"/>
       <c r="P50">
         <v>14</v>
@@ -2792,26 +2792,26 @@
       </c>
     </row>
     <row r="51" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="18" t="s">
+      <c r="B51" s="26"/>
+      <c r="C51" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="D51" s="19"/>
-      <c r="E51" s="18" t="s">
+      <c r="D51" s="20"/>
+      <c r="E51" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="F51" s="20"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="13"/>
-      <c r="I51" s="14"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="15"/>
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
-      <c r="L51" s="13"/>
-      <c r="M51" s="15"/>
-      <c r="N51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="22"/>
+      <c r="N51" s="15"/>
       <c r="O51" s="2"/>
       <c r="P51">
         <v>19</v>
@@ -2821,26 +2821,26 @@
       </c>
     </row>
     <row r="52" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="16" t="s">
+      <c r="A52" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="B52" s="17"/>
-      <c r="C52" s="18" t="s">
+      <c r="B52" s="26"/>
+      <c r="C52" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="D52" s="19"/>
-      <c r="E52" s="18" t="s">
+      <c r="D52" s="20"/>
+      <c r="E52" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="F52" s="20"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="14"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="15"/>
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
-      <c r="L52" s="13"/>
-      <c r="M52" s="15"/>
-      <c r="N52" s="14"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="22"/>
+      <c r="N52" s="15"/>
       <c r="O52" s="2"/>
       <c r="P52">
         <v>13</v>
@@ -2850,26 +2850,26 @@
       </c>
     </row>
     <row r="53" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="B53" s="17"/>
-      <c r="C53" s="18" t="s">
+      <c r="B53" s="26"/>
+      <c r="C53" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="D53" s="19"/>
-      <c r="E53" s="18" t="s">
+      <c r="D53" s="20"/>
+      <c r="E53" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="F53" s="20"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="14"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="15"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
-      <c r="L53" s="13"/>
-      <c r="M53" s="15"/>
-      <c r="N53" s="14"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="22"/>
+      <c r="N53" s="15"/>
       <c r="O53" s="2"/>
       <c r="P53">
         <v>19</v>
@@ -2879,52 +2879,52 @@
       </c>
     </row>
     <row r="54" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="16" t="s">
+      <c r="A54" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="B54" s="17"/>
-      <c r="C54" s="18" t="s">
+      <c r="B54" s="26"/>
+      <c r="C54" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="D54" s="19"/>
-      <c r="E54" s="18" t="s">
+      <c r="D54" s="20"/>
+      <c r="E54" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="F54" s="20"/>
-      <c r="G54" s="19"/>
-      <c r="H54" s="13"/>
-      <c r="I54" s="14"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="15"/>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
-      <c r="L54" s="13"/>
-      <c r="M54" s="15"/>
-      <c r="N54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="22"/>
+      <c r="N54" s="15"/>
       <c r="O54" s="2"/>
       <c r="P54">
         <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="16" t="s">
+      <c r="A55" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="B55" s="17"/>
-      <c r="C55" s="18" t="s">
+      <c r="B55" s="26"/>
+      <c r="C55" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="D55" s="19"/>
-      <c r="E55" s="18" t="s">
+      <c r="D55" s="20"/>
+      <c r="E55" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="F55" s="20"/>
-      <c r="G55" s="19"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="14"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="15"/>
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
-      <c r="L55" s="13"/>
-      <c r="M55" s="15"/>
-      <c r="N55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="22"/>
+      <c r="N55" s="15"/>
       <c r="O55" s="2"/>
       <c r="P55">
         <v>10</v>
@@ -2934,78 +2934,78 @@
       </c>
     </row>
     <row r="56" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="B56" s="17"/>
-      <c r="C56" s="18" t="s">
+      <c r="B56" s="26"/>
+      <c r="C56" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="D56" s="19"/>
-      <c r="E56" s="18" t="s">
+      <c r="D56" s="20"/>
+      <c r="E56" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="F56" s="20"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="14"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="15"/>
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
-      <c r="L56" s="13"/>
-      <c r="M56" s="15"/>
-      <c r="N56" s="14"/>
+      <c r="L56" s="14"/>
+      <c r="M56" s="22"/>
+      <c r="N56" s="15"/>
       <c r="O56" s="2"/>
       <c r="Q56">
         <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="16" t="s">
+      <c r="A57" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="B57" s="17"/>
-      <c r="C57" s="18" t="s">
+      <c r="B57" s="26"/>
+      <c r="C57" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="D57" s="19"/>
-      <c r="E57" s="18" t="s">
+      <c r="D57" s="20"/>
+      <c r="E57" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="F57" s="20"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="14"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="15"/>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
-      <c r="L57" s="13"/>
-      <c r="M57" s="15"/>
-      <c r="N57" s="14"/>
+      <c r="L57" s="14"/>
+      <c r="M57" s="22"/>
+      <c r="N57" s="15"/>
       <c r="O57" s="2"/>
       <c r="P57">
         <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="16" t="s">
+      <c r="A58" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="B58" s="17"/>
-      <c r="C58" s="18" t="s">
+      <c r="B58" s="26"/>
+      <c r="C58" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="D58" s="19"/>
-      <c r="E58" s="18" t="s">
+      <c r="D58" s="20"/>
+      <c r="E58" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="F58" s="20"/>
-      <c r="G58" s="19"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="14"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="15"/>
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
-      <c r="L58" s="13"/>
-      <c r="M58" s="15"/>
-      <c r="N58" s="14"/>
+      <c r="L58" s="14"/>
+      <c r="M58" s="22"/>
+      <c r="N58" s="15"/>
       <c r="O58" s="2"/>
       <c r="P58">
         <v>9</v>
@@ -3015,49 +3015,49 @@
       </c>
     </row>
     <row r="59" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="16" t="s">
+      <c r="A59" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="B59" s="17"/>
-      <c r="C59" s="18" t="s">
+      <c r="B59" s="26"/>
+      <c r="C59" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="D59" s="19"/>
-      <c r="E59" s="18" t="s">
+      <c r="D59" s="20"/>
+      <c r="E59" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="F59" s="20"/>
-      <c r="G59" s="19"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="14"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="15"/>
       <c r="J59" s="5"/>
       <c r="K59" s="5"/>
-      <c r="L59" s="13"/>
-      <c r="M59" s="15"/>
-      <c r="N59" s="14"/>
+      <c r="L59" s="14"/>
+      <c r="M59" s="22"/>
+      <c r="N59" s="15"/>
       <c r="O59" s="2"/>
     </row>
     <row r="60" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="B60" s="17"/>
-      <c r="C60" s="18" t="s">
+      <c r="B60" s="26"/>
+      <c r="C60" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="D60" s="19"/>
-      <c r="E60" s="18" t="s">
+      <c r="D60" s="20"/>
+      <c r="E60" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="F60" s="20"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="13"/>
-      <c r="I60" s="14"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="15"/>
       <c r="J60" s="5"/>
       <c r="K60" s="5"/>
-      <c r="L60" s="13"/>
-      <c r="M60" s="15"/>
-      <c r="N60" s="14"/>
+      <c r="L60" s="14"/>
+      <c r="M60" s="22"/>
+      <c r="N60" s="15"/>
       <c r="O60" s="2"/>
       <c r="P60">
         <v>15</v>
@@ -3067,26 +3067,26 @@
       </c>
     </row>
     <row r="61" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="B61" s="17"/>
-      <c r="C61" s="18" t="s">
+      <c r="B61" s="26"/>
+      <c r="C61" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="D61" s="19"/>
-      <c r="E61" s="18" t="s">
+      <c r="D61" s="20"/>
+      <c r="E61" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="F61" s="20"/>
-      <c r="G61" s="19"/>
-      <c r="H61" s="13"/>
-      <c r="I61" s="14"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="15"/>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
-      <c r="L61" s="13"/>
-      <c r="M61" s="15"/>
-      <c r="N61" s="14"/>
+      <c r="L61" s="14"/>
+      <c r="M61" s="22"/>
+      <c r="N61" s="15"/>
       <c r="O61" s="2"/>
       <c r="P61">
         <v>15</v>
@@ -3096,26 +3096,26 @@
       </c>
     </row>
     <row r="62" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="B62" s="17"/>
-      <c r="C62" s="18" t="s">
+      <c r="B62" s="26"/>
+      <c r="C62" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="D62" s="19"/>
-      <c r="E62" s="18" t="s">
+      <c r="D62" s="20"/>
+      <c r="E62" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="F62" s="20"/>
-      <c r="G62" s="19"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="14"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="15"/>
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
-      <c r="L62" s="13"/>
-      <c r="M62" s="15"/>
-      <c r="N62" s="14"/>
+      <c r="L62" s="14"/>
+      <c r="M62" s="22"/>
+      <c r="N62" s="15"/>
       <c r="O62" s="2"/>
       <c r="P62">
         <v>10</v>
@@ -3125,127 +3125,127 @@
       </c>
     </row>
     <row r="63" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="16" t="s">
+      <c r="A63" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="B63" s="17"/>
-      <c r="C63" s="18" t="s">
+      <c r="B63" s="26"/>
+      <c r="C63" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="D63" s="19"/>
-      <c r="E63" s="18" t="s">
+      <c r="D63" s="20"/>
+      <c r="E63" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="F63" s="20"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="14"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="15"/>
       <c r="J63" s="5"/>
       <c r="K63" s="5"/>
-      <c r="L63" s="13"/>
-      <c r="M63" s="15"/>
-      <c r="N63" s="14"/>
+      <c r="L63" s="14"/>
+      <c r="M63" s="22"/>
+      <c r="N63" s="15"/>
       <c r="O63" s="2"/>
     </row>
     <row r="64" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="B64" s="17"/>
-      <c r="C64" s="18" t="s">
+      <c r="B64" s="26"/>
+      <c r="C64" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="D64" s="19"/>
-      <c r="E64" s="18" t="s">
+      <c r="D64" s="20"/>
+      <c r="E64" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="F64" s="20"/>
-      <c r="G64" s="19"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="14"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="15"/>
       <c r="J64" s="5"/>
       <c r="K64" s="5"/>
-      <c r="L64" s="13"/>
-      <c r="M64" s="15"/>
-      <c r="N64" s="14"/>
+      <c r="L64" s="14"/>
+      <c r="M64" s="22"/>
+      <c r="N64" s="15"/>
       <c r="O64" s="2"/>
       <c r="Q64">
         <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="16" t="s">
+      <c r="A65" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="B65" s="17"/>
-      <c r="C65" s="18" t="s">
+      <c r="B65" s="26"/>
+      <c r="C65" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="D65" s="19"/>
-      <c r="E65" s="18" t="s">
+      <c r="D65" s="20"/>
+      <c r="E65" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="F65" s="20"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="14"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="15"/>
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
-      <c r="L65" s="13"/>
-      <c r="M65" s="15"/>
-      <c r="N65" s="14"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="22"/>
+      <c r="N65" s="15"/>
       <c r="O65" s="2"/>
       <c r="P65">
         <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="16" t="s">
+      <c r="A66" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="B66" s="17"/>
-      <c r="C66" s="18" t="s">
+      <c r="B66" s="26"/>
+      <c r="C66" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="D66" s="19"/>
-      <c r="E66" s="18" t="s">
+      <c r="D66" s="20"/>
+      <c r="E66" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="F66" s="20"/>
-      <c r="G66" s="19"/>
-      <c r="H66" s="13"/>
-      <c r="I66" s="14"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="15"/>
       <c r="J66" s="5"/>
       <c r="K66" s="5"/>
-      <c r="L66" s="13"/>
-      <c r="M66" s="15"/>
-      <c r="N66" s="14"/>
+      <c r="L66" s="14"/>
+      <c r="M66" s="22"/>
+      <c r="N66" s="15"/>
       <c r="O66" s="2"/>
       <c r="Q66">
         <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="16" t="s">
+      <c r="A67" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="B67" s="17"/>
-      <c r="C67" s="18" t="s">
+      <c r="B67" s="26"/>
+      <c r="C67" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="D67" s="19"/>
-      <c r="E67" s="18" t="s">
+      <c r="D67" s="20"/>
+      <c r="E67" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="F67" s="20"/>
-      <c r="G67" s="19"/>
-      <c r="H67" s="13"/>
-      <c r="I67" s="14"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="20"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="15"/>
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
-      <c r="L67" s="13"/>
-      <c r="M67" s="15"/>
-      <c r="N67" s="14"/>
+      <c r="L67" s="14"/>
+      <c r="M67" s="22"/>
+      <c r="N67" s="15"/>
       <c r="O67" s="2"/>
       <c r="P67">
         <v>20</v>
@@ -3255,26 +3255,26 @@
       </c>
     </row>
     <row r="68" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="16" t="s">
+      <c r="A68" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="B68" s="17"/>
-      <c r="C68" s="18" t="s">
+      <c r="B68" s="26"/>
+      <c r="C68" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="D68" s="19"/>
-      <c r="E68" s="18" t="s">
+      <c r="D68" s="20"/>
+      <c r="E68" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="F68" s="20"/>
-      <c r="G68" s="19"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="14"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="20"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="15"/>
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
-      <c r="L68" s="13"/>
-      <c r="M68" s="15"/>
-      <c r="N68" s="14"/>
+      <c r="L68" s="14"/>
+      <c r="M68" s="22"/>
+      <c r="N68" s="15"/>
       <c r="O68" s="2"/>
       <c r="P68">
         <v>14</v>
@@ -3284,26 +3284,26 @@
       </c>
     </row>
     <row r="69" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="25" t="s">
         <v>205</v>
       </c>
-      <c r="B69" s="17"/>
-      <c r="C69" s="18" t="s">
+      <c r="B69" s="26"/>
+      <c r="C69" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="D69" s="19"/>
-      <c r="E69" s="18" t="s">
+      <c r="D69" s="20"/>
+      <c r="E69" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="F69" s="20"/>
-      <c r="G69" s="19"/>
-      <c r="H69" s="13"/>
-      <c r="I69" s="14"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="20"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="15"/>
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
-      <c r="L69" s="13"/>
-      <c r="M69" s="15"/>
-      <c r="N69" s="14"/>
+      <c r="L69" s="14"/>
+      <c r="M69" s="22"/>
+      <c r="N69" s="15"/>
       <c r="O69" s="2"/>
       <c r="P69">
         <v>15</v>
@@ -3313,52 +3313,52 @@
       </c>
     </row>
     <row r="70" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="16" t="s">
+      <c r="A70" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="B70" s="17"/>
-      <c r="C70" s="18" t="s">
+      <c r="B70" s="26"/>
+      <c r="C70" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="D70" s="19"/>
-      <c r="E70" s="18" t="s">
+      <c r="D70" s="20"/>
+      <c r="E70" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="F70" s="20"/>
-      <c r="G70" s="19"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="14"/>
+      <c r="F70" s="21"/>
+      <c r="G70" s="20"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="15"/>
       <c r="J70" s="5"/>
       <c r="K70" s="5"/>
-      <c r="L70" s="13"/>
-      <c r="M70" s="15"/>
-      <c r="N70" s="14"/>
+      <c r="L70" s="14"/>
+      <c r="M70" s="22"/>
+      <c r="N70" s="15"/>
       <c r="O70" s="2"/>
       <c r="P70">
         <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="16" t="s">
+      <c r="A71" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="B71" s="17"/>
-      <c r="C71" s="18" t="s">
+      <c r="B71" s="26"/>
+      <c r="C71" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="D71" s="19"/>
-      <c r="E71" s="18" t="s">
+      <c r="D71" s="20"/>
+      <c r="E71" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="F71" s="20"/>
-      <c r="G71" s="19"/>
-      <c r="H71" s="13"/>
-      <c r="I71" s="14"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="20"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="15"/>
       <c r="J71" s="5"/>
       <c r="K71" s="5"/>
-      <c r="L71" s="13"/>
-      <c r="M71" s="15"/>
-      <c r="N71" s="14"/>
+      <c r="L71" s="14"/>
+      <c r="M71" s="22"/>
+      <c r="N71" s="15"/>
       <c r="O71" s="2"/>
       <c r="P71">
         <v>16</v>
@@ -3368,26 +3368,26 @@
       </c>
     </row>
     <row r="72" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="16" t="s">
+      <c r="A72" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="B72" s="17"/>
-      <c r="C72" s="18" t="s">
+      <c r="B72" s="26"/>
+      <c r="C72" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="D72" s="19"/>
-      <c r="E72" s="18" t="s">
+      <c r="D72" s="20"/>
+      <c r="E72" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="F72" s="20"/>
-      <c r="G72" s="19"/>
-      <c r="H72" s="13"/>
-      <c r="I72" s="14"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="20"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="15"/>
       <c r="J72" s="5"/>
       <c r="K72" s="5"/>
-      <c r="L72" s="13"/>
-      <c r="M72" s="15"/>
-      <c r="N72" s="14"/>
+      <c r="L72" s="14"/>
+      <c r="M72" s="22"/>
+      <c r="N72" s="15"/>
       <c r="O72" s="2"/>
       <c r="P72">
         <v>17</v>
@@ -3397,26 +3397,26 @@
       </c>
     </row>
     <row r="73" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="16" t="s">
+      <c r="A73" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="B73" s="17"/>
-      <c r="C73" s="18" t="s">
+      <c r="B73" s="26"/>
+      <c r="C73" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="D73" s="19"/>
-      <c r="E73" s="18" t="s">
+      <c r="D73" s="20"/>
+      <c r="E73" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="F73" s="20"/>
-      <c r="G73" s="19"/>
-      <c r="H73" s="13"/>
-      <c r="I73" s="14"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="20"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="15"/>
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
-      <c r="L73" s="13"/>
-      <c r="M73" s="15"/>
-      <c r="N73" s="14"/>
+      <c r="L73" s="14"/>
+      <c r="M73" s="22"/>
+      <c r="N73" s="15"/>
       <c r="O73" s="2"/>
       <c r="P73">
         <v>12</v>
@@ -3426,505 +3426,505 @@
       </c>
     </row>
     <row r="74" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="16" t="s">
+      <c r="A74" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="B74" s="17"/>
-      <c r="C74" s="18" t="s">
+      <c r="B74" s="26"/>
+      <c r="C74" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="D74" s="19"/>
-      <c r="E74" s="18" t="s">
+      <c r="D74" s="20"/>
+      <c r="E74" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="F74" s="20"/>
-      <c r="G74" s="19"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="14"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="20"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="15"/>
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
-      <c r="L74" s="13"/>
-      <c r="M74" s="15"/>
-      <c r="N74" s="14"/>
+      <c r="L74" s="14"/>
+      <c r="M74" s="22"/>
+      <c r="N74" s="15"/>
       <c r="O74" s="2"/>
       <c r="P74">
         <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="11"/>
-      <c r="B75" s="11"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12"/>
-      <c r="E75" s="12"/>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="13"/>
-      <c r="I75" s="14"/>
+      <c r="A75" s="30"/>
+      <c r="B75" s="30"/>
+      <c r="C75" s="31"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="31"/>
+      <c r="F75" s="31"/>
+      <c r="G75" s="31"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="15"/>
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
-      <c r="L75" s="13"/>
-      <c r="M75" s="15"/>
-      <c r="N75" s="14"/>
+      <c r="L75" s="14"/>
+      <c r="M75" s="22"/>
+      <c r="N75" s="15"/>
       <c r="O75" s="2"/>
     </row>
     <row r="76" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="11"/>
-      <c r="B76" s="11"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
-      <c r="E76" s="12"/>
-      <c r="F76" s="12"/>
-      <c r="G76" s="12"/>
-      <c r="H76" s="13"/>
-      <c r="I76" s="14"/>
+      <c r="A76" s="30"/>
+      <c r="B76" s="30"/>
+      <c r="C76" s="31"/>
+      <c r="D76" s="31"/>
+      <c r="E76" s="31"/>
+      <c r="F76" s="31"/>
+      <c r="G76" s="31"/>
+      <c r="H76" s="14"/>
+      <c r="I76" s="15"/>
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
-      <c r="L76" s="13"/>
-      <c r="M76" s="15"/>
-      <c r="N76" s="14"/>
+      <c r="L76" s="14"/>
+      <c r="M76" s="22"/>
+      <c r="N76" s="15"/>
       <c r="O76" s="2"/>
     </row>
     <row r="77" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="11"/>
-      <c r="B77" s="11"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="12"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="13"/>
-      <c r="I77" s="14"/>
+      <c r="A77" s="30"/>
+      <c r="B77" s="30"/>
+      <c r="C77" s="31"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="31"/>
+      <c r="F77" s="31"/>
+      <c r="G77" s="31"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="15"/>
       <c r="J77" s="5"/>
       <c r="K77" s="5"/>
-      <c r="L77" s="13"/>
-      <c r="M77" s="15"/>
-      <c r="N77" s="14"/>
+      <c r="L77" s="14"/>
+      <c r="M77" s="22"/>
+      <c r="N77" s="15"/>
       <c r="O77" s="2"/>
     </row>
     <row r="78" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="11"/>
-      <c r="B78" s="11"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="13"/>
-      <c r="I78" s="14"/>
+      <c r="A78" s="30"/>
+      <c r="B78" s="30"/>
+      <c r="C78" s="31"/>
+      <c r="D78" s="31"/>
+      <c r="E78" s="31"/>
+      <c r="F78" s="31"/>
+      <c r="G78" s="31"/>
+      <c r="H78" s="14"/>
+      <c r="I78" s="15"/>
       <c r="J78" s="5"/>
       <c r="K78" s="5"/>
-      <c r="L78" s="13"/>
-      <c r="M78" s="15"/>
-      <c r="N78" s="14"/>
+      <c r="L78" s="14"/>
+      <c r="M78" s="22"/>
+      <c r="N78" s="15"/>
       <c r="O78" s="2"/>
     </row>
     <row r="79" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="11"/>
-      <c r="B79" s="11"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="13"/>
-      <c r="I79" s="14"/>
+      <c r="A79" s="30"/>
+      <c r="B79" s="30"/>
+      <c r="C79" s="31"/>
+      <c r="D79" s="31"/>
+      <c r="E79" s="31"/>
+      <c r="F79" s="31"/>
+      <c r="G79" s="31"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="15"/>
       <c r="J79" s="5"/>
       <c r="K79" s="5"/>
-      <c r="L79" s="13"/>
-      <c r="M79" s="15"/>
-      <c r="N79" s="14"/>
+      <c r="L79" s="14"/>
+      <c r="M79" s="22"/>
+      <c r="N79" s="15"/>
       <c r="O79" s="2"/>
     </row>
     <row r="80" spans="1:17" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="11"/>
-      <c r="B80" s="11"/>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
-      <c r="G80" s="12"/>
-      <c r="H80" s="13"/>
-      <c r="I80" s="14"/>
+      <c r="A80" s="30"/>
+      <c r="B80" s="30"/>
+      <c r="C80" s="31"/>
+      <c r="D80" s="31"/>
+      <c r="E80" s="31"/>
+      <c r="F80" s="31"/>
+      <c r="G80" s="31"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="15"/>
       <c r="J80" s="5"/>
       <c r="K80" s="5"/>
-      <c r="L80" s="13"/>
-      <c r="M80" s="15"/>
-      <c r="N80" s="14"/>
+      <c r="L80" s="14"/>
+      <c r="M80" s="22"/>
+      <c r="N80" s="15"/>
       <c r="O80" s="2"/>
     </row>
     <row r="81" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="11"/>
-      <c r="B81" s="11"/>
-      <c r="C81" s="12"/>
-      <c r="D81" s="12"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
-      <c r="H81" s="13"/>
-      <c r="I81" s="14"/>
+      <c r="A81" s="30"/>
+      <c r="B81" s="30"/>
+      <c r="C81" s="31"/>
+      <c r="D81" s="31"/>
+      <c r="E81" s="31"/>
+      <c r="F81" s="31"/>
+      <c r="G81" s="31"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="15"/>
       <c r="J81" s="5"/>
       <c r="K81" s="5"/>
-      <c r="L81" s="13"/>
-      <c r="M81" s="15"/>
-      <c r="N81" s="14"/>
+      <c r="L81" s="14"/>
+      <c r="M81" s="22"/>
+      <c r="N81" s="15"/>
       <c r="O81" s="2"/>
     </row>
     <row r="82" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="11"/>
-      <c r="B82" s="11"/>
-      <c r="C82" s="12"/>
-      <c r="D82" s="12"/>
-      <c r="E82" s="12"/>
-      <c r="F82" s="12"/>
-      <c r="G82" s="12"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="14"/>
+      <c r="A82" s="30"/>
+      <c r="B82" s="30"/>
+      <c r="C82" s="31"/>
+      <c r="D82" s="31"/>
+      <c r="E82" s="31"/>
+      <c r="F82" s="31"/>
+      <c r="G82" s="31"/>
+      <c r="H82" s="14"/>
+      <c r="I82" s="15"/>
       <c r="J82" s="5"/>
       <c r="K82" s="5"/>
-      <c r="L82" s="13"/>
-      <c r="M82" s="15"/>
-      <c r="N82" s="14"/>
+      <c r="L82" s="14"/>
+      <c r="M82" s="22"/>
+      <c r="N82" s="15"/>
       <c r="O82" s="2"/>
     </row>
     <row r="83" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="11"/>
-      <c r="B83" s="11"/>
-      <c r="C83" s="12"/>
-      <c r="D83" s="12"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="12"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="13"/>
-      <c r="I83" s="14"/>
+      <c r="A83" s="30"/>
+      <c r="B83" s="30"/>
+      <c r="C83" s="31"/>
+      <c r="D83" s="31"/>
+      <c r="E83" s="31"/>
+      <c r="F83" s="31"/>
+      <c r="G83" s="31"/>
+      <c r="H83" s="14"/>
+      <c r="I83" s="15"/>
       <c r="J83" s="5"/>
       <c r="K83" s="5"/>
-      <c r="L83" s="13"/>
-      <c r="M83" s="15"/>
-      <c r="N83" s="14"/>
+      <c r="L83" s="14"/>
+      <c r="M83" s="22"/>
+      <c r="N83" s="15"/>
       <c r="O83" s="2"/>
     </row>
     <row r="84" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="11"/>
-      <c r="B84" s="11"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="14"/>
+      <c r="A84" s="30"/>
+      <c r="B84" s="30"/>
+      <c r="C84" s="31"/>
+      <c r="D84" s="31"/>
+      <c r="E84" s="31"/>
+      <c r="F84" s="31"/>
+      <c r="G84" s="31"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="15"/>
       <c r="J84" s="5"/>
       <c r="K84" s="5"/>
-      <c r="L84" s="13"/>
-      <c r="M84" s="15"/>
-      <c r="N84" s="14"/>
+      <c r="L84" s="14"/>
+      <c r="M84" s="22"/>
+      <c r="N84" s="15"/>
       <c r="O84" s="2"/>
     </row>
     <row r="85" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="11"/>
-      <c r="B85" s="11"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
-      <c r="E85" s="12"/>
-      <c r="F85" s="12"/>
-      <c r="G85" s="12"/>
-      <c r="H85" s="13"/>
-      <c r="I85" s="14"/>
+      <c r="A85" s="30"/>
+      <c r="B85" s="30"/>
+      <c r="C85" s="31"/>
+      <c r="D85" s="31"/>
+      <c r="E85" s="31"/>
+      <c r="F85" s="31"/>
+      <c r="G85" s="31"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="15"/>
       <c r="J85" s="5"/>
       <c r="K85" s="5"/>
-      <c r="L85" s="13"/>
-      <c r="M85" s="15"/>
-      <c r="N85" s="14"/>
+      <c r="L85" s="14"/>
+      <c r="M85" s="22"/>
+      <c r="N85" s="15"/>
       <c r="O85" s="2"/>
     </row>
     <row r="86" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="11"/>
-      <c r="B86" s="11"/>
-      <c r="C86" s="12"/>
-      <c r="D86" s="12"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="12"/>
-      <c r="G86" s="12"/>
-      <c r="H86" s="13"/>
-      <c r="I86" s="14"/>
+      <c r="A86" s="30"/>
+      <c r="B86" s="30"/>
+      <c r="C86" s="31"/>
+      <c r="D86" s="31"/>
+      <c r="E86" s="31"/>
+      <c r="F86" s="31"/>
+      <c r="G86" s="31"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="15"/>
       <c r="J86" s="5"/>
       <c r="K86" s="5"/>
-      <c r="L86" s="13"/>
-      <c r="M86" s="15"/>
-      <c r="N86" s="14"/>
+      <c r="L86" s="14"/>
+      <c r="M86" s="22"/>
+      <c r="N86" s="15"/>
       <c r="O86" s="2"/>
     </row>
     <row r="87" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="11"/>
-      <c r="B87" s="11"/>
-      <c r="C87" s="12"/>
-      <c r="D87" s="12"/>
-      <c r="E87" s="12"/>
-      <c r="F87" s="12"/>
-      <c r="G87" s="12"/>
-      <c r="H87" s="13"/>
-      <c r="I87" s="14"/>
+      <c r="A87" s="30"/>
+      <c r="B87" s="30"/>
+      <c r="C87" s="31"/>
+      <c r="D87" s="31"/>
+      <c r="E87" s="31"/>
+      <c r="F87" s="31"/>
+      <c r="G87" s="31"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="15"/>
       <c r="J87" s="5"/>
       <c r="K87" s="5"/>
-      <c r="L87" s="13"/>
-      <c r="M87" s="15"/>
-      <c r="N87" s="14"/>
+      <c r="L87" s="14"/>
+      <c r="M87" s="22"/>
+      <c r="N87" s="15"/>
       <c r="O87" s="2"/>
     </row>
     <row r="88" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="11"/>
-      <c r="B88" s="11"/>
-      <c r="C88" s="12"/>
-      <c r="D88" s="12"/>
-      <c r="E88" s="12"/>
-      <c r="F88" s="12"/>
-      <c r="G88" s="12"/>
-      <c r="H88" s="13"/>
-      <c r="I88" s="14"/>
+      <c r="A88" s="30"/>
+      <c r="B88" s="30"/>
+      <c r="C88" s="31"/>
+      <c r="D88" s="31"/>
+      <c r="E88" s="31"/>
+      <c r="F88" s="31"/>
+      <c r="G88" s="31"/>
+      <c r="H88" s="14"/>
+      <c r="I88" s="15"/>
       <c r="J88" s="5"/>
       <c r="K88" s="5"/>
-      <c r="L88" s="13"/>
-      <c r="M88" s="15"/>
-      <c r="N88" s="14"/>
+      <c r="L88" s="14"/>
+      <c r="M88" s="22"/>
+      <c r="N88" s="15"/>
       <c r="O88" s="2"/>
     </row>
     <row r="89" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="11"/>
-      <c r="B89" s="11"/>
-      <c r="C89" s="12"/>
-      <c r="D89" s="12"/>
-      <c r="E89" s="12"/>
-      <c r="F89" s="12"/>
-      <c r="G89" s="12"/>
-      <c r="H89" s="13"/>
-      <c r="I89" s="14"/>
+      <c r="A89" s="30"/>
+      <c r="B89" s="30"/>
+      <c r="C89" s="31"/>
+      <c r="D89" s="31"/>
+      <c r="E89" s="31"/>
+      <c r="F89" s="31"/>
+      <c r="G89" s="31"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="15"/>
       <c r="J89" s="5"/>
       <c r="K89" s="5"/>
-      <c r="L89" s="13"/>
-      <c r="M89" s="15"/>
-      <c r="N89" s="14"/>
+      <c r="L89" s="14"/>
+      <c r="M89" s="22"/>
+      <c r="N89" s="15"/>
       <c r="O89" s="2"/>
     </row>
     <row r="90" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="11"/>
-      <c r="B90" s="11"/>
-      <c r="C90" s="12"/>
-      <c r="D90" s="12"/>
-      <c r="E90" s="12"/>
-      <c r="F90" s="12"/>
-      <c r="G90" s="12"/>
-      <c r="H90" s="13"/>
-      <c r="I90" s="14"/>
+      <c r="A90" s="30"/>
+      <c r="B90" s="30"/>
+      <c r="C90" s="31"/>
+      <c r="D90" s="31"/>
+      <c r="E90" s="31"/>
+      <c r="F90" s="31"/>
+      <c r="G90" s="31"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="15"/>
       <c r="J90" s="5"/>
       <c r="K90" s="5"/>
-      <c r="L90" s="13"/>
-      <c r="M90" s="15"/>
-      <c r="N90" s="14"/>
+      <c r="L90" s="14"/>
+      <c r="M90" s="22"/>
+      <c r="N90" s="15"/>
       <c r="O90" s="2"/>
     </row>
     <row r="91" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="11"/>
-      <c r="B91" s="11"/>
-      <c r="C91" s="12"/>
-      <c r="D91" s="12"/>
-      <c r="E91" s="12"/>
-      <c r="F91" s="12"/>
-      <c r="G91" s="12"/>
-      <c r="H91" s="13"/>
-      <c r="I91" s="14"/>
+      <c r="A91" s="30"/>
+      <c r="B91" s="30"/>
+      <c r="C91" s="31"/>
+      <c r="D91" s="31"/>
+      <c r="E91" s="31"/>
+      <c r="F91" s="31"/>
+      <c r="G91" s="31"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="15"/>
       <c r="J91" s="5"/>
       <c r="K91" s="5"/>
-      <c r="L91" s="13"/>
-      <c r="M91" s="15"/>
-      <c r="N91" s="14"/>
+      <c r="L91" s="14"/>
+      <c r="M91" s="22"/>
+      <c r="N91" s="15"/>
       <c r="O91" s="2"/>
     </row>
     <row r="92" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="11"/>
-      <c r="B92" s="11"/>
-      <c r="C92" s="12"/>
-      <c r="D92" s="12"/>
-      <c r="E92" s="12"/>
-      <c r="F92" s="12"/>
-      <c r="G92" s="12"/>
-      <c r="H92" s="13"/>
-      <c r="I92" s="14"/>
+      <c r="A92" s="30"/>
+      <c r="B92" s="30"/>
+      <c r="C92" s="31"/>
+      <c r="D92" s="31"/>
+      <c r="E92" s="31"/>
+      <c r="F92" s="31"/>
+      <c r="G92" s="31"/>
+      <c r="H92" s="14"/>
+      <c r="I92" s="15"/>
       <c r="J92" s="5"/>
       <c r="K92" s="5"/>
-      <c r="L92" s="13"/>
-      <c r="M92" s="15"/>
-      <c r="N92" s="14"/>
+      <c r="L92" s="14"/>
+      <c r="M92" s="22"/>
+      <c r="N92" s="15"/>
       <c r="O92" s="2"/>
     </row>
     <row r="93" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="11"/>
-      <c r="B93" s="11"/>
-      <c r="C93" s="12"/>
-      <c r="D93" s="12"/>
-      <c r="E93" s="12"/>
-      <c r="F93" s="12"/>
-      <c r="G93" s="12"/>
-      <c r="H93" s="13"/>
-      <c r="I93" s="14"/>
+      <c r="A93" s="30"/>
+      <c r="B93" s="30"/>
+      <c r="C93" s="31"/>
+      <c r="D93" s="31"/>
+      <c r="E93" s="31"/>
+      <c r="F93" s="31"/>
+      <c r="G93" s="31"/>
+      <c r="H93" s="14"/>
+      <c r="I93" s="15"/>
       <c r="J93" s="5"/>
       <c r="K93" s="5"/>
-      <c r="L93" s="13"/>
-      <c r="M93" s="15"/>
-      <c r="N93" s="14"/>
+      <c r="L93" s="14"/>
+      <c r="M93" s="22"/>
+      <c r="N93" s="15"/>
       <c r="O93" s="2"/>
     </row>
     <row r="94" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="11"/>
-      <c r="B94" s="11"/>
-      <c r="C94" s="12"/>
-      <c r="D94" s="12"/>
-      <c r="E94" s="12"/>
-      <c r="F94" s="12"/>
-      <c r="G94" s="12"/>
-      <c r="H94" s="13"/>
-      <c r="I94" s="14"/>
+      <c r="A94" s="30"/>
+      <c r="B94" s="30"/>
+      <c r="C94" s="31"/>
+      <c r="D94" s="31"/>
+      <c r="E94" s="31"/>
+      <c r="F94" s="31"/>
+      <c r="G94" s="31"/>
+      <c r="H94" s="14"/>
+      <c r="I94" s="15"/>
       <c r="J94" s="5"/>
       <c r="K94" s="5"/>
-      <c r="L94" s="13"/>
-      <c r="M94" s="15"/>
-      <c r="N94" s="14"/>
+      <c r="L94" s="14"/>
+      <c r="M94" s="22"/>
+      <c r="N94" s="15"/>
       <c r="O94" s="2"/>
     </row>
     <row r="95" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="11"/>
-      <c r="B95" s="11"/>
-      <c r="C95" s="12"/>
-      <c r="D95" s="12"/>
-      <c r="E95" s="12"/>
-      <c r="F95" s="12"/>
-      <c r="G95" s="12"/>
-      <c r="H95" s="13"/>
-      <c r="I95" s="14"/>
+      <c r="A95" s="30"/>
+      <c r="B95" s="30"/>
+      <c r="C95" s="31"/>
+      <c r="D95" s="31"/>
+      <c r="E95" s="31"/>
+      <c r="F95" s="31"/>
+      <c r="G95" s="31"/>
+      <c r="H95" s="14"/>
+      <c r="I95" s="15"/>
       <c r="J95" s="5"/>
       <c r="K95" s="5"/>
-      <c r="L95" s="13"/>
-      <c r="M95" s="15"/>
-      <c r="N95" s="14"/>
+      <c r="L95" s="14"/>
+      <c r="M95" s="22"/>
+      <c r="N95" s="15"/>
       <c r="O95" s="2"/>
     </row>
     <row r="96" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="11"/>
-      <c r="B96" s="11"/>
-      <c r="C96" s="12"/>
-      <c r="D96" s="12"/>
-      <c r="E96" s="12"/>
-      <c r="F96" s="12"/>
-      <c r="G96" s="12"/>
-      <c r="H96" s="13"/>
-      <c r="I96" s="14"/>
+      <c r="A96" s="30"/>
+      <c r="B96" s="30"/>
+      <c r="C96" s="31"/>
+      <c r="D96" s="31"/>
+      <c r="E96" s="31"/>
+      <c r="F96" s="31"/>
+      <c r="G96" s="31"/>
+      <c r="H96" s="14"/>
+      <c r="I96" s="15"/>
       <c r="J96" s="5"/>
       <c r="K96" s="5"/>
-      <c r="L96" s="13"/>
-      <c r="M96" s="15"/>
-      <c r="N96" s="14"/>
+      <c r="L96" s="14"/>
+      <c r="M96" s="22"/>
+      <c r="N96" s="15"/>
       <c r="O96" s="2"/>
     </row>
     <row r="97" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="11"/>
-      <c r="B97" s="11"/>
-      <c r="C97" s="12"/>
-      <c r="D97" s="12"/>
-      <c r="E97" s="12"/>
-      <c r="F97" s="12"/>
-      <c r="G97" s="12"/>
-      <c r="H97" s="13"/>
-      <c r="I97" s="14"/>
+      <c r="A97" s="30"/>
+      <c r="B97" s="30"/>
+      <c r="C97" s="31"/>
+      <c r="D97" s="31"/>
+      <c r="E97" s="31"/>
+      <c r="F97" s="31"/>
+      <c r="G97" s="31"/>
+      <c r="H97" s="14"/>
+      <c r="I97" s="15"/>
       <c r="J97" s="5"/>
       <c r="K97" s="5"/>
-      <c r="L97" s="13"/>
-      <c r="M97" s="15"/>
-      <c r="N97" s="14"/>
+      <c r="L97" s="14"/>
+      <c r="M97" s="22"/>
+      <c r="N97" s="15"/>
       <c r="O97" s="2"/>
     </row>
     <row r="98" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="11"/>
-      <c r="B98" s="11"/>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12"/>
-      <c r="E98" s="12"/>
-      <c r="F98" s="12"/>
-      <c r="G98" s="12"/>
-      <c r="H98" s="13"/>
-      <c r="I98" s="14"/>
+      <c r="A98" s="30"/>
+      <c r="B98" s="30"/>
+      <c r="C98" s="31"/>
+      <c r="D98" s="31"/>
+      <c r="E98" s="31"/>
+      <c r="F98" s="31"/>
+      <c r="G98" s="31"/>
+      <c r="H98" s="14"/>
+      <c r="I98" s="15"/>
       <c r="J98" s="5"/>
       <c r="K98" s="5"/>
-      <c r="L98" s="13"/>
-      <c r="M98" s="15"/>
-      <c r="N98" s="14"/>
+      <c r="L98" s="14"/>
+      <c r="M98" s="22"/>
+      <c r="N98" s="15"/>
       <c r="O98" s="2"/>
     </row>
     <row r="99" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="11"/>
-      <c r="B99" s="11"/>
-      <c r="C99" s="12"/>
-      <c r="D99" s="12"/>
-      <c r="E99" s="12"/>
-      <c r="F99" s="12"/>
-      <c r="G99" s="12"/>
-      <c r="H99" s="13"/>
-      <c r="I99" s="14"/>
+      <c r="A99" s="30"/>
+      <c r="B99" s="30"/>
+      <c r="C99" s="31"/>
+      <c r="D99" s="31"/>
+      <c r="E99" s="31"/>
+      <c r="F99" s="31"/>
+      <c r="G99" s="31"/>
+      <c r="H99" s="14"/>
+      <c r="I99" s="15"/>
       <c r="J99" s="5"/>
       <c r="K99" s="5"/>
-      <c r="L99" s="13"/>
-      <c r="M99" s="15"/>
-      <c r="N99" s="14"/>
+      <c r="L99" s="14"/>
+      <c r="M99" s="22"/>
+      <c r="N99" s="15"/>
       <c r="O99" s="2"/>
     </row>
     <row r="100" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="11"/>
-      <c r="B100" s="11"/>
-      <c r="C100" s="12"/>
-      <c r="D100" s="12"/>
-      <c r="E100" s="12"/>
-      <c r="F100" s="12"/>
-      <c r="G100" s="12"/>
-      <c r="H100" s="13"/>
-      <c r="I100" s="14"/>
+      <c r="A100" s="30"/>
+      <c r="B100" s="30"/>
+      <c r="C100" s="31"/>
+      <c r="D100" s="31"/>
+      <c r="E100" s="31"/>
+      <c r="F100" s="31"/>
+      <c r="G100" s="31"/>
+      <c r="H100" s="14"/>
+      <c r="I100" s="15"/>
       <c r="J100" s="5"/>
       <c r="K100" s="5"/>
-      <c r="L100" s="13"/>
-      <c r="M100" s="15"/>
-      <c r="N100" s="14"/>
+      <c r="L100" s="14"/>
+      <c r="M100" s="22"/>
+      <c r="N100" s="15"/>
       <c r="O100" s="2"/>
     </row>
     <row r="101" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="11"/>
-      <c r="B101" s="11"/>
-      <c r="C101" s="12"/>
-      <c r="D101" s="12"/>
-      <c r="E101" s="12"/>
-      <c r="F101" s="12"/>
-      <c r="G101" s="12"/>
-      <c r="H101" s="13"/>
-      <c r="I101" s="14"/>
+      <c r="A101" s="30"/>
+      <c r="B101" s="30"/>
+      <c r="C101" s="31"/>
+      <c r="D101" s="31"/>
+      <c r="E101" s="31"/>
+      <c r="F101" s="31"/>
+      <c r="G101" s="31"/>
+      <c r="H101" s="14"/>
+      <c r="I101" s="15"/>
       <c r="J101" s="5"/>
       <c r="K101" s="5"/>
-      <c r="L101" s="13"/>
-      <c r="M101" s="15"/>
-      <c r="N101" s="14"/>
+      <c r="L101" s="14"/>
+      <c r="M101" s="22"/>
+      <c r="N101" s="15"/>
       <c r="O101" s="2"/>
     </row>
     <row r="102" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="11"/>
-      <c r="B102" s="11"/>
-      <c r="C102" s="12"/>
-      <c r="D102" s="12"/>
-      <c r="E102" s="12"/>
-      <c r="F102" s="12"/>
-      <c r="G102" s="12"/>
-      <c r="H102" s="13"/>
-      <c r="I102" s="14"/>
+      <c r="A102" s="30"/>
+      <c r="B102" s="30"/>
+      <c r="C102" s="31"/>
+      <c r="D102" s="31"/>
+      <c r="E102" s="31"/>
+      <c r="F102" s="31"/>
+      <c r="G102" s="31"/>
+      <c r="H102" s="14"/>
+      <c r="I102" s="15"/>
       <c r="J102" s="5"/>
       <c r="K102" s="5"/>
-      <c r="L102" s="13"/>
-      <c r="M102" s="15"/>
-      <c r="N102" s="14"/>
+      <c r="L102" s="14"/>
+      <c r="M102" s="22"/>
+      <c r="N102" s="15"/>
       <c r="O102" s="2"/>
     </row>
   </sheetData>
@@ -3938,39 +3938,431 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="482">
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:M4"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="I7:M7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="E102:G102"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="L102:N102"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="E96:G96"/>
+    <mergeCell ref="H96:I96"/>
+    <mergeCell ref="L96:N96"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="E100:G100"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="L100:N100"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="E98:G98"/>
+    <mergeCell ref="H98:I98"/>
+    <mergeCell ref="L98:N98"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="E101:G101"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="L101:N101"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="E94:G94"/>
+    <mergeCell ref="H94:I94"/>
+    <mergeCell ref="L94:N94"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="E99:G99"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="L99:N99"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="E95:G95"/>
+    <mergeCell ref="H95:I95"/>
+    <mergeCell ref="L95:N95"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="E93:G93"/>
+    <mergeCell ref="H93:I93"/>
+    <mergeCell ref="L93:N93"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="E97:G97"/>
+    <mergeCell ref="H97:I97"/>
+    <mergeCell ref="L97:N97"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="E91:G91"/>
+    <mergeCell ref="H91:I91"/>
+    <mergeCell ref="L91:N91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="E92:G92"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="L92:N92"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="E89:G89"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="L89:N89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="E90:G90"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="L90:N90"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="E87:G87"/>
+    <mergeCell ref="H87:I87"/>
+    <mergeCell ref="L87:N87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="E88:G88"/>
+    <mergeCell ref="H88:I88"/>
+    <mergeCell ref="L88:N88"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="E85:G85"/>
+    <mergeCell ref="H85:I85"/>
+    <mergeCell ref="L85:N85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="E86:G86"/>
+    <mergeCell ref="H86:I86"/>
+    <mergeCell ref="L86:N86"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="E83:G83"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="L83:N83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="E84:G84"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="L84:N84"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="E81:G81"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="L81:N81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="E82:G82"/>
+    <mergeCell ref="H82:I82"/>
+    <mergeCell ref="L82:N82"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="H79:I79"/>
+    <mergeCell ref="L79:N79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="L80:N80"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="E78:G78"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="L78:N78"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="L76:N76"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="L77:N77"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="E75:G75"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="L75:N75"/>
+    <mergeCell ref="L74:N74"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="L68:N68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="L69:N69"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="L72:N72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="L73:N73"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="L70:N70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="L71:N71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="L66:N66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="L67:N67"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="L64:N64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="L65:N65"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="L62:N62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="L63:N63"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="L60:N60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="L61:N61"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="L58:N58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="L59:N59"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="L56:N56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="L57:N57"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="L54:N54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="L55:N55"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="L52:N52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="L53:N53"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="L50:N50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="L51:N51"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="L48:N48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="L49:N49"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="L46:N46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="L47:N47"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="L44:N44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="L45:N45"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="L43:N43"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="L38:N38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="L41:N41"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="L39:N39"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="L36:N36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="L37:N37"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="L35:N35"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="L32:N32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="L33:N33"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="L30:N30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="L28:N28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="L29:N29"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="L26:N26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="L21:N21"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="L19:N19"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:F3"/>
@@ -3995,431 +4387,39 @@
     <mergeCell ref="L12:N12"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="L20:N20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="L21:N21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="L23:N23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="L24:N24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="L25:N25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="L26:N26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="L28:N28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="L29:N29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="L32:N32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="L33:N33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="L35:N35"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="L39:N39"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="L36:N36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="L37:N37"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="L43:N43"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="L38:N38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="L41:N41"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="L44:N44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="L45:N45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="L46:N46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="L47:N47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="L48:N48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="L49:N49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="L50:N50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="L51:N51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="L52:N52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="L53:N53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="L54:N54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="L55:N55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="L56:N56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="L57:N57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="L58:N58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="L59:N59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="L60:N60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="L61:N61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="L62:N62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="L63:N63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="L64:N64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="L65:N65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="L66:N66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="L67:N67"/>
-    <mergeCell ref="E72:G72"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="L72:N72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="H73:I73"/>
-    <mergeCell ref="L73:N73"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="L68:N68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="L69:N69"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="L70:N70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="L71:N71"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="E77:G77"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="L77:N77"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="L75:N75"/>
-    <mergeCell ref="L74:N74"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="E78:G78"/>
-    <mergeCell ref="H78:I78"/>
-    <mergeCell ref="L78:N78"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="L76:N76"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="E79:G79"/>
-    <mergeCell ref="H79:I79"/>
-    <mergeCell ref="L79:N79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="H80:I80"/>
-    <mergeCell ref="L80:N80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="E81:G81"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="L81:N81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="E82:G82"/>
-    <mergeCell ref="H82:I82"/>
-    <mergeCell ref="L82:N82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="E83:G83"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="L83:N83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="E84:G84"/>
-    <mergeCell ref="H84:I84"/>
-    <mergeCell ref="L84:N84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="E85:G85"/>
-    <mergeCell ref="H85:I85"/>
-    <mergeCell ref="L85:N85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="E86:G86"/>
-    <mergeCell ref="H86:I86"/>
-    <mergeCell ref="L86:N86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="E87:G87"/>
-    <mergeCell ref="H87:I87"/>
-    <mergeCell ref="L87:N87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="E88:G88"/>
-    <mergeCell ref="H88:I88"/>
-    <mergeCell ref="L88:N88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="E89:G89"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="L89:N89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="E90:G90"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="L90:N90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="E91:G91"/>
-    <mergeCell ref="H91:I91"/>
-    <mergeCell ref="L91:N91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="E92:G92"/>
-    <mergeCell ref="H92:I92"/>
-    <mergeCell ref="L92:N92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="E93:G93"/>
-    <mergeCell ref="H93:I93"/>
-    <mergeCell ref="L93:N93"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="E97:G97"/>
-    <mergeCell ref="H97:I97"/>
-    <mergeCell ref="L97:N97"/>
-    <mergeCell ref="L101:N101"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="E94:G94"/>
-    <mergeCell ref="H94:I94"/>
-    <mergeCell ref="L94:N94"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="E99:G99"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="L99:N99"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="E95:G95"/>
-    <mergeCell ref="H95:I95"/>
-    <mergeCell ref="L95:N95"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="E102:G102"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="L102:N102"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="E96:G96"/>
-    <mergeCell ref="H96:I96"/>
-    <mergeCell ref="L96:N96"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="E100:G100"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="L100:N100"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="E98:G98"/>
-    <mergeCell ref="H98:I98"/>
-    <mergeCell ref="L98:N98"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="E101:G101"/>
-    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:M4"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <pageMargins left="0.39" right="0.39" top="0.39" bottom="0.39" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update, aun no corrijo los examenes ni las practicas
</commit_message>
<xml_diff>
--- a/OYM/_Documentos Comunes/BD_C32017.xlsx
+++ b/OYM/_Documentos Comunes/BD_C32017.xlsx
@@ -918,13 +918,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -933,14 +930,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -951,23 +948,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
@@ -975,10 +969,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1365,9 +1365,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z24" sqref="Z24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X34" sqref="X34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1398,19 +1398,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -1431,19 +1431,19 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
       <c r="N3" s="2"/>
       <c r="P3" t="s">
         <v>21</v>
@@ -1453,19 +1453,19 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
       <c r="N4" s="2"/>
       <c r="P4" t="s">
         <v>23</v>
@@ -1475,19 +1475,19 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
       <c r="N5" s="2"/>
       <c r="P5" t="s">
         <v>25</v>
@@ -1519,19 +1519,19 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
       <c r="N7" s="2"/>
       <c r="P7" t="s">
         <v>29</v>
@@ -1585,10 +1585,10 @@
       <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:26" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="23"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="24" t="s">
         <v>2</v>
       </c>
@@ -1598,21 +1598,21 @@
       </c>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="23"/>
+      <c r="I10" s="25"/>
       <c r="J10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="23" t="s">
+      <c r="L10" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
       <c r="O10" s="2"/>
       <c r="P10" t="s">
         <v>8</v>
@@ -1649,35 +1649,35 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28">
+      <c r="A11" s="26">
         <v>0</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="11" t="s">
+      <c r="B11" s="27"/>
+      <c r="C11" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="11" t="s">
+      <c r="D11" s="29"/>
+      <c r="E11" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="14">
+      <c r="F11" s="30"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="13">
         <v>10</v>
       </c>
-      <c r="I11" s="15"/>
+      <c r="I11" s="14"/>
       <c r="J11" s="5">
         <v>20</v>
       </c>
       <c r="K11" s="5">
         <v>20</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="13">
         <f>IF((Y11-50)&gt;50,50,IF((Y11-50)&lt;0,0,(Y11-50)))</f>
         <v>50</v>
       </c>
-      <c r="M11" s="22"/>
-      <c r="N11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="14"/>
       <c r="O11" s="2"/>
       <c r="P11">
         <v>20</v>
@@ -1715,26 +1715,26 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="19" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="19" t="s">
+      <c r="D12" s="19"/>
+      <c r="E12" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="15"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="14"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="15"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="14"/>
       <c r="O12" s="2"/>
       <c r="P12">
         <v>12</v>
@@ -1760,26 +1760,26 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="19" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="19" t="s">
+      <c r="D13" s="19"/>
+      <c r="E13" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="15"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="14"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="15"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="14"/>
       <c r="O13" s="2"/>
       <c r="P13">
         <v>10</v>
@@ -1805,26 +1805,26 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="19" t="s">
+      <c r="B14" s="17"/>
+      <c r="C14" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="19" t="s">
+      <c r="D14" s="19"/>
+      <c r="E14" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="15"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="14"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="15"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="14"/>
       <c r="O14" s="2"/>
       <c r="Y14">
         <f t="shared" si="0"/>
@@ -1835,26 +1835,26 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="19" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="19" t="s">
+      <c r="D15" s="19"/>
+      <c r="E15" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="15"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="14"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="15"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="14"/>
       <c r="O15" s="2"/>
       <c r="P15">
         <v>8</v>
@@ -1880,26 +1880,26 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="19" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="19" t="s">
+      <c r="D16" s="19"/>
+      <c r="E16" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="15"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="14"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="15"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="14"/>
       <c r="O16" s="2"/>
       <c r="P16">
         <v>10</v>
@@ -1925,26 +1925,26 @@
       </c>
     </row>
     <row r="17" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="19" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="19" t="s">
+      <c r="D17" s="19"/>
+      <c r="E17" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="15"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="14"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="15"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="14"/>
       <c r="O17" s="2"/>
       <c r="P17">
         <v>17</v>
@@ -1967,26 +1967,26 @@
       </c>
     </row>
     <row r="18" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="19" t="s">
+      <c r="B18" s="17"/>
+      <c r="C18" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="19" t="s">
+      <c r="D18" s="19"/>
+      <c r="E18" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="15"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="14"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="15"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="14"/>
       <c r="O18" s="2"/>
       <c r="Q18">
         <v>2</v>
@@ -2003,26 +2003,26 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="19" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="19" t="s">
+      <c r="D19" s="19"/>
+      <c r="E19" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="15"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="14"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="15"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="14"/>
       <c r="O19" s="2"/>
       <c r="P19">
         <v>15</v>
@@ -2039,26 +2039,26 @@
       </c>
     </row>
     <row r="20" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="19" t="s">
+      <c r="B20" s="17"/>
+      <c r="C20" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="19" t="s">
+      <c r="D20" s="19"/>
+      <c r="E20" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="15"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="14"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="15"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="14"/>
       <c r="O20" s="2"/>
       <c r="P20">
         <v>11</v>
@@ -2084,26 +2084,26 @@
       </c>
     </row>
     <row r="21" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="19" t="s">
+      <c r="B21" s="17"/>
+      <c r="C21" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="19" t="s">
+      <c r="D21" s="19"/>
+      <c r="E21" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="15"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="14"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="15"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="14"/>
       <c r="O21" s="2"/>
       <c r="P21">
         <v>11</v>
@@ -2120,26 +2120,26 @@
       </c>
     </row>
     <row r="22" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="19" t="s">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="19" t="s">
+      <c r="D22" s="19"/>
+      <c r="E22" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="15"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="14"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="15"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="14"/>
       <c r="O22" s="2"/>
       <c r="P22">
         <v>8</v>
@@ -2168,26 +2168,26 @@
       </c>
     </row>
     <row r="23" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="19" t="s">
+      <c r="B23" s="17"/>
+      <c r="C23" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="19" t="s">
+      <c r="D23" s="19"/>
+      <c r="E23" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="15"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="14"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="15"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="14"/>
       <c r="O23" s="2"/>
       <c r="Y23">
         <f t="shared" si="0"/>
@@ -2198,26 +2198,26 @@
       </c>
     </row>
     <row r="24" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="19" t="s">
+      <c r="B24" s="17"/>
+      <c r="C24" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="19" t="s">
+      <c r="D24" s="19"/>
+      <c r="E24" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="15"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="14"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="15"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="14"/>
       <c r="O24" s="2"/>
       <c r="P24">
         <v>16</v>
@@ -2246,26 +2246,26 @@
       </c>
     </row>
     <row r="25" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="19" t="s">
+      <c r="B25" s="17"/>
+      <c r="C25" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="19" t="s">
+      <c r="D25" s="19"/>
+      <c r="E25" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="15"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="14"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="15"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="14"/>
       <c r="O25" s="2"/>
       <c r="P25">
         <v>16</v>
@@ -2294,26 +2294,26 @@
       </c>
     </row>
     <row r="26" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="19" t="s">
+      <c r="B26" s="17"/>
+      <c r="C26" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="19" t="s">
+      <c r="D26" s="19"/>
+      <c r="E26" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="15"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="14"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="15"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="14"/>
       <c r="O26" s="2"/>
       <c r="P26">
         <v>10</v>
@@ -2339,26 +2339,26 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="19" t="s">
+      <c r="B27" s="17"/>
+      <c r="C27" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="19" t="s">
+      <c r="D27" s="19"/>
+      <c r="E27" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="15"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="14"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="15"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="14"/>
       <c r="O27" s="2"/>
       <c r="P27">
         <v>12</v>
@@ -2384,26 +2384,26 @@
       </c>
     </row>
     <row r="28" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="19" t="s">
+      <c r="B28" s="17"/>
+      <c r="C28" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="19" t="s">
+      <c r="D28" s="19"/>
+      <c r="E28" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="15"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="14"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="15"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="14"/>
       <c r="O28" s="2"/>
       <c r="P28">
         <v>11</v>
@@ -2429,26 +2429,26 @@
       </c>
     </row>
     <row r="29" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="19" t="s">
+      <c r="B29" s="17"/>
+      <c r="C29" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="19" t="s">
+      <c r="D29" s="19"/>
+      <c r="E29" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="15"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="14"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="15"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="14"/>
       <c r="O29" s="2"/>
       <c r="P29">
         <v>13</v>
@@ -2477,26 +2477,26 @@
       </c>
     </row>
     <row r="30" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="19" t="s">
+      <c r="B30" s="17"/>
+      <c r="C30" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="20"/>
-      <c r="E30" s="19" t="s">
+      <c r="D30" s="19"/>
+      <c r="E30" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F30" s="21"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="15"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="14"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="15"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="14"/>
       <c r="O30" s="2"/>
       <c r="P30">
         <v>11</v>
@@ -2522,26 +2522,26 @@
       </c>
     </row>
     <row r="31" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="19" t="s">
+      <c r="B31" s="17"/>
+      <c r="C31" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="20"/>
-      <c r="E31" s="19" t="s">
+      <c r="D31" s="19"/>
+      <c r="E31" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="F31" s="21"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="15"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="14"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="15"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="14"/>
       <c r="O31" s="2"/>
       <c r="Y31">
         <f t="shared" si="0"/>
@@ -2552,26 +2552,26 @@
       </c>
     </row>
     <row r="32" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="19" t="s">
+      <c r="B32" s="17"/>
+      <c r="C32" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D32" s="20"/>
-      <c r="E32" s="19" t="s">
+      <c r="D32" s="19"/>
+      <c r="E32" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="F32" s="21"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="15"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="14"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="15"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="14"/>
       <c r="O32" s="2"/>
       <c r="P32">
         <v>10</v>
@@ -2594,26 +2594,26 @@
       </c>
     </row>
     <row r="33" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="19" t="s">
+      <c r="B33" s="17"/>
+      <c r="C33" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D33" s="20"/>
-      <c r="E33" s="19" t="s">
+      <c r="D33" s="19"/>
+      <c r="E33" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="F33" s="21"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="15"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="14"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="15"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="14"/>
       <c r="O33" s="2"/>
       <c r="P33">
         <v>10</v>
@@ -2639,26 +2639,26 @@
       </c>
     </row>
     <row r="34" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="19" t="s">
+      <c r="B34" s="17"/>
+      <c r="C34" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="19" t="s">
+      <c r="D34" s="19"/>
+      <c r="E34" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="F34" s="21"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="15"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="14"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="15"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="14"/>
       <c r="O34" s="2"/>
       <c r="P34">
         <v>9</v>
@@ -2666,35 +2666,38 @@
       <c r="Q34">
         <v>6</v>
       </c>
+      <c r="X34">
+        <v>30</v>
+      </c>
       <c r="Y34">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="Z34">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B35" s="26"/>
-      <c r="C35" s="19" t="s">
+      <c r="B35" s="17"/>
+      <c r="C35" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="19" t="s">
+      <c r="D35" s="19"/>
+      <c r="E35" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="F35" s="21"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="15"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="14"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="15"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="14"/>
       <c r="O35" s="2"/>
       <c r="P35">
         <v>9</v>
@@ -2702,35 +2705,38 @@
       <c r="Q35">
         <v>9</v>
       </c>
+      <c r="X35">
+        <v>30</v>
+      </c>
       <c r="Y35">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="Z35">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B36" s="26"/>
-      <c r="C36" s="19" t="s">
+      <c r="B36" s="17"/>
+      <c r="C36" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D36" s="20"/>
-      <c r="E36" s="19" t="s">
+      <c r="D36" s="19"/>
+      <c r="E36" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="F36" s="21"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="15"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="14"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="15"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="14"/>
       <c r="O36" s="2"/>
       <c r="P36">
         <v>10</v>
@@ -2756,26 +2762,26 @@
       </c>
     </row>
     <row r="37" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="26"/>
-      <c r="C37" s="19" t="s">
+      <c r="B37" s="17"/>
+      <c r="C37" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="20"/>
-      <c r="E37" s="19" t="s">
+      <c r="D37" s="19"/>
+      <c r="E37" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="F37" s="21"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="15"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="14"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="15"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="14"/>
       <c r="O37" s="2"/>
       <c r="P37">
         <v>12</v>
@@ -2789,26 +2795,26 @@
       </c>
     </row>
     <row r="38" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="B38" s="26"/>
-      <c r="C38" s="19" t="s">
+      <c r="B38" s="17"/>
+      <c r="C38" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="20"/>
-      <c r="E38" s="19" t="s">
+      <c r="D38" s="19"/>
+      <c r="E38" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="F38" s="21"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="15"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="14"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="15"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="14"/>
       <c r="O38" s="2"/>
       <c r="P38">
         <v>8</v>
@@ -2834,26 +2840,26 @@
       </c>
     </row>
     <row r="39" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="26"/>
-      <c r="C39" s="19" t="s">
+      <c r="B39" s="17"/>
+      <c r="C39" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="20"/>
-      <c r="E39" s="19" t="s">
+      <c r="D39" s="19"/>
+      <c r="E39" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="F39" s="21"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="15"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="14"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="15"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="14"/>
       <c r="O39" s="2"/>
       <c r="P39">
         <v>8</v>
@@ -2870,26 +2876,26 @@
       </c>
     </row>
     <row r="40" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="19" t="s">
+      <c r="B40" s="17"/>
+      <c r="C40" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="20"/>
-      <c r="E40" s="19" t="s">
+      <c r="D40" s="19"/>
+      <c r="E40" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F40" s="21"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="15"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="14"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="15"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="14"/>
       <c r="O40" s="2"/>
       <c r="P40">
         <v>15</v>
@@ -2918,26 +2924,26 @@
       </c>
     </row>
     <row r="41" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="B41" s="26"/>
-      <c r="C41" s="19" t="s">
+      <c r="B41" s="17"/>
+      <c r="C41" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="19" t="s">
+      <c r="D41" s="19"/>
+      <c r="E41" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="F41" s="21"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="15"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="14"/>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="15"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="14"/>
       <c r="O41" s="2"/>
       <c r="P41">
         <v>10</v>
@@ -2963,26 +2969,26 @@
       </c>
     </row>
     <row r="42" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B42" s="26"/>
-      <c r="C42" s="19" t="s">
+      <c r="B42" s="17"/>
+      <c r="C42" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="19" t="s">
+      <c r="D42" s="19"/>
+      <c r="E42" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="F42" s="21"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="15"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="14"/>
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="15"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="14"/>
       <c r="O42" s="2"/>
       <c r="P42">
         <v>12</v>
@@ -3011,26 +3017,26 @@
       </c>
     </row>
     <row r="43" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="26"/>
-      <c r="C43" s="19" t="s">
+      <c r="B43" s="17"/>
+      <c r="C43" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="19" t="s">
+      <c r="D43" s="19"/>
+      <c r="E43" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="F43" s="21"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="15"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="14"/>
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="15"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="14"/>
       <c r="O43" s="2"/>
       <c r="P43">
         <v>17</v>
@@ -3059,26 +3065,26 @@
       </c>
     </row>
     <row r="44" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="B44" s="26"/>
-      <c r="C44" s="19" t="s">
+      <c r="B44" s="17"/>
+      <c r="C44" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="D44" s="20"/>
-      <c r="E44" s="19" t="s">
+      <c r="D44" s="19"/>
+      <c r="E44" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="F44" s="21"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="15"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="14"/>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="15"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="14"/>
       <c r="O44" s="2"/>
       <c r="P44">
         <v>10</v>
@@ -3104,26 +3110,26 @@
       </c>
     </row>
     <row r="45" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B45" s="26"/>
-      <c r="C45" s="19" t="s">
+      <c r="B45" s="17"/>
+      <c r="C45" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="19" t="s">
+      <c r="D45" s="19"/>
+      <c r="E45" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="F45" s="21"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="15"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="14"/>
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="22"/>
-      <c r="N45" s="15"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="14"/>
       <c r="O45" s="2"/>
       <c r="P45">
         <v>19</v>
@@ -3152,26 +3158,26 @@
       </c>
     </row>
     <row r="46" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="25" t="s">
+      <c r="A46" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="B46" s="26"/>
-      <c r="C46" s="19" t="s">
+      <c r="B46" s="17"/>
+      <c r="C46" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="D46" s="20"/>
-      <c r="E46" s="19" t="s">
+      <c r="D46" s="19"/>
+      <c r="E46" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="F46" s="21"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="15"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="14"/>
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="22"/>
-      <c r="N46" s="15"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="14"/>
       <c r="O46" s="2"/>
       <c r="P46">
         <v>10</v>
@@ -3197,26 +3203,26 @@
       </c>
     </row>
     <row r="47" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="B47" s="26"/>
-      <c r="C47" s="19" t="s">
+      <c r="B47" s="17"/>
+      <c r="C47" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="19" t="s">
+      <c r="D47" s="19"/>
+      <c r="E47" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="F47" s="21"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="15"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="14"/>
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="22"/>
-      <c r="N47" s="15"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="14"/>
       <c r="O47" s="2"/>
       <c r="Q47">
         <v>7</v>
@@ -3242,26 +3248,26 @@
       </c>
     </row>
     <row r="48" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B48" s="26"/>
-      <c r="C48" s="19" t="s">
+      <c r="B48" s="17"/>
+      <c r="C48" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="19" t="s">
+      <c r="D48" s="19"/>
+      <c r="E48" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="F48" s="21"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="15"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="14"/>
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="22"/>
-      <c r="N48" s="15"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="14"/>
       <c r="O48" s="2"/>
       <c r="P48">
         <v>20</v>
@@ -3281,26 +3287,26 @@
       </c>
     </row>
     <row r="49" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="B49" s="26"/>
-      <c r="C49" s="19" t="s">
+      <c r="B49" s="17"/>
+      <c r="C49" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="D49" s="20"/>
-      <c r="E49" s="19" t="s">
+      <c r="D49" s="19"/>
+      <c r="E49" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="F49" s="21"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="15"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="14"/>
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="22"/>
-      <c r="N49" s="15"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="14"/>
       <c r="O49" s="2"/>
       <c r="P49">
         <v>17</v>
@@ -3320,26 +3326,26 @@
       </c>
     </row>
     <row r="50" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="25" t="s">
+      <c r="A50" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="B50" s="26"/>
-      <c r="C50" s="19" t="s">
+      <c r="B50" s="17"/>
+      <c r="C50" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="D50" s="20"/>
-      <c r="E50" s="19" t="s">
+      <c r="D50" s="19"/>
+      <c r="E50" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="F50" s="21"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="15"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="14"/>
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="22"/>
-      <c r="N50" s="15"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="15"/>
+      <c r="N50" s="14"/>
       <c r="O50" s="2"/>
       <c r="P50">
         <v>14</v>
@@ -3365,26 +3371,26 @@
       </c>
     </row>
     <row r="51" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="25" t="s">
+      <c r="A51" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="B51" s="26"/>
-      <c r="C51" s="19" t="s">
+      <c r="B51" s="17"/>
+      <c r="C51" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="D51" s="20"/>
-      <c r="E51" s="19" t="s">
+      <c r="D51" s="19"/>
+      <c r="E51" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="F51" s="21"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="15"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="14"/>
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="22"/>
-      <c r="N51" s="15"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="14"/>
       <c r="O51" s="2"/>
       <c r="P51">
         <v>19</v>
@@ -3404,26 +3410,26 @@
       </c>
     </row>
     <row r="52" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="25" t="s">
+      <c r="A52" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="B52" s="26"/>
-      <c r="C52" s="19" t="s">
+      <c r="B52" s="17"/>
+      <c r="C52" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="D52" s="20"/>
-      <c r="E52" s="19" t="s">
+      <c r="D52" s="19"/>
+      <c r="E52" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="F52" s="21"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="15"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="14"/>
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="22"/>
-      <c r="N52" s="15"/>
+      <c r="L52" s="13"/>
+      <c r="M52" s="15"/>
+      <c r="N52" s="14"/>
       <c r="O52" s="2"/>
       <c r="P52">
         <v>13</v>
@@ -3449,26 +3455,26 @@
       </c>
     </row>
     <row r="53" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="25" t="s">
+      <c r="A53" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="B53" s="26"/>
-      <c r="C53" s="19" t="s">
+      <c r="B53" s="17"/>
+      <c r="C53" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="D53" s="20"/>
-      <c r="E53" s="19" t="s">
+      <c r="D53" s="19"/>
+      <c r="E53" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="F53" s="21"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="15"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="14"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="22"/>
-      <c r="N53" s="15"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="14"/>
       <c r="O53" s="2"/>
       <c r="P53">
         <v>19</v>
@@ -3497,26 +3503,26 @@
       </c>
     </row>
     <row r="54" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="25" t="s">
+      <c r="A54" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="B54" s="26"/>
-      <c r="C54" s="19" t="s">
+      <c r="B54" s="17"/>
+      <c r="C54" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="D54" s="20"/>
-      <c r="E54" s="19" t="s">
+      <c r="D54" s="19"/>
+      <c r="E54" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="F54" s="21"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="15"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="14"/>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="22"/>
-      <c r="N54" s="15"/>
+      <c r="L54" s="13"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="14"/>
       <c r="O54" s="2"/>
       <c r="P54">
         <v>14</v>
@@ -3539,26 +3545,26 @@
       </c>
     </row>
     <row r="55" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="25" t="s">
+      <c r="A55" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="B55" s="26"/>
-      <c r="C55" s="19" t="s">
+      <c r="B55" s="17"/>
+      <c r="C55" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="D55" s="20"/>
-      <c r="E55" s="19" t="s">
+      <c r="D55" s="19"/>
+      <c r="E55" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="F55" s="21"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="15"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="14"/>
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="22"/>
-      <c r="N55" s="15"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="14"/>
       <c r="O55" s="2"/>
       <c r="P55">
         <v>10</v>
@@ -3584,26 +3590,26 @@
       </c>
     </row>
     <row r="56" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="B56" s="26"/>
-      <c r="C56" s="19" t="s">
+      <c r="B56" s="17"/>
+      <c r="C56" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="D56" s="20"/>
-      <c r="E56" s="19" t="s">
+      <c r="D56" s="19"/>
+      <c r="E56" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="F56" s="21"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="15"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="14"/>
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
-      <c r="L56" s="14"/>
-      <c r="M56" s="22"/>
-      <c r="N56" s="15"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="15"/>
+      <c r="N56" s="14"/>
       <c r="O56" s="2"/>
       <c r="Q56">
         <v>8</v>
@@ -3626,26 +3632,26 @@
       </c>
     </row>
     <row r="57" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="25" t="s">
+      <c r="A57" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="B57" s="26"/>
-      <c r="C57" s="19" t="s">
+      <c r="B57" s="17"/>
+      <c r="C57" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="D57" s="20"/>
-      <c r="E57" s="19" t="s">
+      <c r="D57" s="19"/>
+      <c r="E57" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="F57" s="21"/>
-      <c r="G57" s="20"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="15"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="14"/>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
-      <c r="L57" s="14"/>
-      <c r="M57" s="22"/>
-      <c r="N57" s="15"/>
+      <c r="L57" s="13"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="14"/>
       <c r="O57" s="2"/>
       <c r="P57">
         <v>10</v>
@@ -3668,26 +3674,26 @@
       </c>
     </row>
     <row r="58" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="25" t="s">
+      <c r="A58" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="B58" s="26"/>
-      <c r="C58" s="19" t="s">
+      <c r="B58" s="17"/>
+      <c r="C58" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="D58" s="20"/>
-      <c r="E58" s="19" t="s">
+      <c r="D58" s="19"/>
+      <c r="E58" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="F58" s="21"/>
-      <c r="G58" s="20"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="15"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="14"/>
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
-      <c r="L58" s="14"/>
-      <c r="M58" s="22"/>
-      <c r="N58" s="15"/>
+      <c r="L58" s="13"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="14"/>
       <c r="O58" s="2"/>
       <c r="P58">
         <v>9</v>
@@ -3713,26 +3719,26 @@
       </c>
     </row>
     <row r="59" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="25" t="s">
+      <c r="A59" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="B59" s="26"/>
-      <c r="C59" s="19" t="s">
+      <c r="B59" s="17"/>
+      <c r="C59" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="D59" s="20"/>
-      <c r="E59" s="19" t="s">
+      <c r="D59" s="19"/>
+      <c r="E59" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="F59" s="21"/>
-      <c r="G59" s="20"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="15"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="14"/>
       <c r="J59" s="5"/>
       <c r="K59" s="5"/>
-      <c r="L59" s="14"/>
-      <c r="M59" s="22"/>
-      <c r="N59" s="15"/>
+      <c r="L59" s="13"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="14"/>
       <c r="O59" s="2"/>
       <c r="U59">
         <v>14</v>
@@ -3752,26 +3758,26 @@
       </c>
     </row>
     <row r="60" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="25" t="s">
+      <c r="A60" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B60" s="26"/>
-      <c r="C60" s="19" t="s">
+      <c r="B60" s="17"/>
+      <c r="C60" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="D60" s="20"/>
-      <c r="E60" s="19" t="s">
+      <c r="D60" s="19"/>
+      <c r="E60" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="F60" s="21"/>
-      <c r="G60" s="20"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="15"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="14"/>
       <c r="J60" s="5"/>
       <c r="K60" s="5"/>
-      <c r="L60" s="14"/>
-      <c r="M60" s="22"/>
-      <c r="N60" s="15"/>
+      <c r="L60" s="13"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="14"/>
       <c r="O60" s="2"/>
       <c r="P60">
         <v>15</v>
@@ -3797,26 +3803,26 @@
       </c>
     </row>
     <row r="61" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="25" t="s">
+      <c r="A61" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="B61" s="26"/>
-      <c r="C61" s="19" t="s">
+      <c r="B61" s="17"/>
+      <c r="C61" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="D61" s="20"/>
-      <c r="E61" s="19" t="s">
+      <c r="D61" s="19"/>
+      <c r="E61" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="F61" s="21"/>
-      <c r="G61" s="20"/>
-      <c r="H61" s="14"/>
-      <c r="I61" s="15"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="14"/>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
-      <c r="L61" s="14"/>
-      <c r="M61" s="22"/>
-      <c r="N61" s="15"/>
+      <c r="L61" s="13"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="14"/>
       <c r="O61" s="2"/>
       <c r="P61">
         <v>15</v>
@@ -3842,26 +3848,26 @@
       </c>
     </row>
     <row r="62" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="25" t="s">
+      <c r="A62" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="B62" s="26"/>
-      <c r="C62" s="19" t="s">
+      <c r="B62" s="17"/>
+      <c r="C62" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="D62" s="20"/>
-      <c r="E62" s="19" t="s">
+      <c r="D62" s="19"/>
+      <c r="E62" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="F62" s="21"/>
-      <c r="G62" s="20"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="15"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="14"/>
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
-      <c r="L62" s="14"/>
-      <c r="M62" s="22"/>
-      <c r="N62" s="15"/>
+      <c r="L62" s="13"/>
+      <c r="M62" s="15"/>
+      <c r="N62" s="14"/>
       <c r="O62" s="2"/>
       <c r="P62">
         <v>10</v>
@@ -3887,26 +3893,26 @@
       </c>
     </row>
     <row r="63" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="25" t="s">
+      <c r="A63" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="B63" s="26"/>
-      <c r="C63" s="19" t="s">
+      <c r="B63" s="17"/>
+      <c r="C63" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="D63" s="20"/>
-      <c r="E63" s="19" t="s">
+      <c r="D63" s="19"/>
+      <c r="E63" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="F63" s="21"/>
-      <c r="G63" s="20"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="15"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="14"/>
       <c r="J63" s="5"/>
       <c r="K63" s="5"/>
-      <c r="L63" s="14"/>
-      <c r="M63" s="22"/>
-      <c r="N63" s="15"/>
+      <c r="L63" s="13"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="14"/>
       <c r="O63" s="2"/>
       <c r="Y63">
         <f t="shared" si="0"/>
@@ -3917,26 +3923,26 @@
       </c>
     </row>
     <row r="64" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="25" t="s">
+      <c r="A64" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="B64" s="26"/>
-      <c r="C64" s="19" t="s">
+      <c r="B64" s="17"/>
+      <c r="C64" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="D64" s="20"/>
-      <c r="E64" s="19" t="s">
+      <c r="D64" s="19"/>
+      <c r="E64" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="F64" s="21"/>
-      <c r="G64" s="20"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="15"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="14"/>
       <c r="J64" s="5"/>
       <c r="K64" s="5"/>
-      <c r="L64" s="14"/>
-      <c r="M64" s="22"/>
-      <c r="N64" s="15"/>
+      <c r="L64" s="13"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="14"/>
       <c r="O64" s="2"/>
       <c r="Q64">
         <v>6</v>
@@ -3950,26 +3956,26 @@
       </c>
     </row>
     <row r="65" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="25" t="s">
+      <c r="A65" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B65" s="26"/>
-      <c r="C65" s="19" t="s">
+      <c r="B65" s="17"/>
+      <c r="C65" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="D65" s="20"/>
-      <c r="E65" s="19" t="s">
+      <c r="D65" s="19"/>
+      <c r="E65" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="F65" s="21"/>
-      <c r="G65" s="20"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="15"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="14"/>
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
-      <c r="L65" s="14"/>
-      <c r="M65" s="22"/>
-      <c r="N65" s="15"/>
+      <c r="L65" s="13"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="14"/>
       <c r="O65" s="2"/>
       <c r="P65">
         <v>9</v>
@@ -3983,35 +3989,38 @@
       <c r="W65">
         <v>14</v>
       </c>
+      <c r="X65">
+        <v>30</v>
+      </c>
       <c r="Y65">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="Z65">
         <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="25" t="s">
+      <c r="A66" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="B66" s="26"/>
-      <c r="C66" s="19" t="s">
+      <c r="B66" s="17"/>
+      <c r="C66" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="D66" s="20"/>
-      <c r="E66" s="19" t="s">
+      <c r="D66" s="19"/>
+      <c r="E66" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="F66" s="21"/>
-      <c r="G66" s="20"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="15"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="14"/>
       <c r="J66" s="5"/>
       <c r="K66" s="5"/>
-      <c r="L66" s="14"/>
-      <c r="M66" s="22"/>
-      <c r="N66" s="15"/>
+      <c r="L66" s="13"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="14"/>
       <c r="O66" s="2"/>
       <c r="Q66">
         <v>8</v>
@@ -4037,26 +4046,26 @@
       </c>
     </row>
     <row r="67" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="25" t="s">
+      <c r="A67" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="B67" s="26"/>
-      <c r="C67" s="19" t="s">
+      <c r="B67" s="17"/>
+      <c r="C67" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="D67" s="20"/>
-      <c r="E67" s="19" t="s">
+      <c r="D67" s="19"/>
+      <c r="E67" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="F67" s="21"/>
-      <c r="G67" s="20"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="15"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="14"/>
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
-      <c r="L67" s="14"/>
-      <c r="M67" s="22"/>
-      <c r="N67" s="15"/>
+      <c r="L67" s="13"/>
+      <c r="M67" s="15"/>
+      <c r="N67" s="14"/>
       <c r="O67" s="2"/>
       <c r="P67">
         <v>20</v>
@@ -4085,26 +4094,26 @@
       </c>
     </row>
     <row r="68" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="25" t="s">
+      <c r="A68" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="B68" s="26"/>
-      <c r="C68" s="19" t="s">
+      <c r="B68" s="17"/>
+      <c r="C68" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="D68" s="20"/>
-      <c r="E68" s="19" t="s">
+      <c r="D68" s="19"/>
+      <c r="E68" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="F68" s="21"/>
-      <c r="G68" s="20"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="15"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="19"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="14"/>
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
-      <c r="L68" s="14"/>
-      <c r="M68" s="22"/>
-      <c r="N68" s="15"/>
+      <c r="L68" s="13"/>
+      <c r="M68" s="15"/>
+      <c r="N68" s="14"/>
       <c r="O68" s="2"/>
       <c r="P68">
         <v>14</v>
@@ -4130,26 +4139,26 @@
       </c>
     </row>
     <row r="69" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="25" t="s">
+      <c r="A69" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="B69" s="26"/>
-      <c r="C69" s="19" t="s">
+      <c r="B69" s="17"/>
+      <c r="C69" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="D69" s="20"/>
-      <c r="E69" s="19" t="s">
+      <c r="D69" s="19"/>
+      <c r="E69" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="F69" s="21"/>
-      <c r="G69" s="20"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="15"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="19"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="14"/>
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
-      <c r="L69" s="14"/>
-      <c r="M69" s="22"/>
-      <c r="N69" s="15"/>
+      <c r="L69" s="13"/>
+      <c r="M69" s="15"/>
+      <c r="N69" s="14"/>
       <c r="O69" s="2"/>
       <c r="P69">
         <v>15</v>
@@ -4175,26 +4184,26 @@
       </c>
     </row>
     <row r="70" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="25" t="s">
+      <c r="A70" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="B70" s="26"/>
-      <c r="C70" s="19" t="s">
+      <c r="B70" s="17"/>
+      <c r="C70" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="D70" s="20"/>
-      <c r="E70" s="19" t="s">
+      <c r="D70" s="19"/>
+      <c r="E70" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="F70" s="21"/>
-      <c r="G70" s="20"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="15"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="19"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="14"/>
       <c r="J70" s="5"/>
       <c r="K70" s="5"/>
-      <c r="L70" s="14"/>
-      <c r="M70" s="22"/>
-      <c r="N70" s="15"/>
+      <c r="L70" s="13"/>
+      <c r="M70" s="15"/>
+      <c r="N70" s="14"/>
       <c r="O70" s="2"/>
       <c r="P70">
         <v>9</v>
@@ -4217,26 +4226,26 @@
       </c>
     </row>
     <row r="71" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="25" t="s">
+      <c r="A71" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="B71" s="26"/>
-      <c r="C71" s="19" t="s">
+      <c r="B71" s="17"/>
+      <c r="C71" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="D71" s="20"/>
-      <c r="E71" s="19" t="s">
+      <c r="D71" s="19"/>
+      <c r="E71" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="F71" s="21"/>
-      <c r="G71" s="20"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="15"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="19"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="14"/>
       <c r="J71" s="5"/>
       <c r="K71" s="5"/>
-      <c r="L71" s="14"/>
-      <c r="M71" s="22"/>
-      <c r="N71" s="15"/>
+      <c r="L71" s="13"/>
+      <c r="M71" s="15"/>
+      <c r="N71" s="14"/>
       <c r="O71" s="2"/>
       <c r="P71">
         <v>16</v>
@@ -4265,26 +4274,26 @@
       </c>
     </row>
     <row r="72" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="25" t="s">
+      <c r="A72" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="B72" s="26"/>
-      <c r="C72" s="19" t="s">
+      <c r="B72" s="17"/>
+      <c r="C72" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="D72" s="20"/>
-      <c r="E72" s="19" t="s">
+      <c r="D72" s="19"/>
+      <c r="E72" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="F72" s="21"/>
-      <c r="G72" s="20"/>
-      <c r="H72" s="14"/>
-      <c r="I72" s="15"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="19"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="14"/>
       <c r="J72" s="5"/>
       <c r="K72" s="5"/>
-      <c r="L72" s="14"/>
-      <c r="M72" s="22"/>
-      <c r="N72" s="15"/>
+      <c r="L72" s="13"/>
+      <c r="M72" s="15"/>
+      <c r="N72" s="14"/>
       <c r="O72" s="2"/>
       <c r="P72">
         <v>17</v>
@@ -4313,26 +4322,26 @@
       </c>
     </row>
     <row r="73" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="25" t="s">
+      <c r="A73" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="B73" s="26"/>
-      <c r="C73" s="19" t="s">
+      <c r="B73" s="17"/>
+      <c r="C73" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="D73" s="20"/>
-      <c r="E73" s="19" t="s">
+      <c r="D73" s="19"/>
+      <c r="E73" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="F73" s="21"/>
-      <c r="G73" s="20"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="15"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="19"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="14"/>
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
-      <c r="L73" s="14"/>
-      <c r="M73" s="22"/>
-      <c r="N73" s="15"/>
+      <c r="L73" s="13"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="14"/>
       <c r="O73" s="2"/>
       <c r="P73">
         <v>12</v>
@@ -4352,26 +4361,26 @@
       </c>
     </row>
     <row r="74" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="25" t="s">
+      <c r="A74" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="B74" s="26"/>
-      <c r="C74" s="19" t="s">
+      <c r="B74" s="17"/>
+      <c r="C74" s="18" t="s">
         <v>221</v>
       </c>
-      <c r="D74" s="20"/>
-      <c r="E74" s="19" t="s">
+      <c r="D74" s="19"/>
+      <c r="E74" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="F74" s="21"/>
-      <c r="G74" s="20"/>
-      <c r="H74" s="14"/>
-      <c r="I74" s="15"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="14"/>
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
-      <c r="L74" s="14"/>
-      <c r="M74" s="22"/>
-      <c r="N74" s="15"/>
+      <c r="L74" s="13"/>
+      <c r="M74" s="15"/>
+      <c r="N74" s="14"/>
       <c r="O74" s="2"/>
       <c r="P74">
         <v>12</v>
@@ -4394,20 +4403,20 @@
       </c>
     </row>
     <row r="75" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="30"/>
-      <c r="B75" s="30"/>
-      <c r="C75" s="31"/>
-      <c r="D75" s="31"/>
-      <c r="E75" s="31"/>
-      <c r="F75" s="31"/>
-      <c r="G75" s="31"/>
-      <c r="H75" s="14"/>
-      <c r="I75" s="15"/>
+      <c r="A75" s="11"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="14"/>
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
-      <c r="L75" s="14"/>
-      <c r="M75" s="22"/>
-      <c r="N75" s="15"/>
+      <c r="L75" s="13"/>
+      <c r="M75" s="15"/>
+      <c r="N75" s="14"/>
       <c r="O75" s="2"/>
       <c r="Y75">
         <f t="shared" si="0"/>
@@ -4418,20 +4427,20 @@
       </c>
     </row>
     <row r="76" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="30"/>
-      <c r="B76" s="30"/>
-      <c r="C76" s="31"/>
-      <c r="D76" s="31"/>
-      <c r="E76" s="31"/>
-      <c r="F76" s="31"/>
-      <c r="G76" s="31"/>
-      <c r="H76" s="14"/>
-      <c r="I76" s="15"/>
+      <c r="A76" s="11"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="14"/>
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
-      <c r="L76" s="14"/>
-      <c r="M76" s="22"/>
-      <c r="N76" s="15"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="15"/>
+      <c r="N76" s="14"/>
       <c r="O76" s="2"/>
       <c r="Y76">
         <f t="shared" si="0"/>
@@ -4442,20 +4451,20 @@
       </c>
     </row>
     <row r="77" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="30"/>
-      <c r="B77" s="30"/>
-      <c r="C77" s="31"/>
-      <c r="D77" s="31"/>
-      <c r="E77" s="31"/>
-      <c r="F77" s="31"/>
-      <c r="G77" s="31"/>
-      <c r="H77" s="14"/>
-      <c r="I77" s="15"/>
+      <c r="A77" s="11"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="14"/>
       <c r="J77" s="5"/>
       <c r="K77" s="5"/>
-      <c r="L77" s="14"/>
-      <c r="M77" s="22"/>
-      <c r="N77" s="15"/>
+      <c r="L77" s="13"/>
+      <c r="M77" s="15"/>
+      <c r="N77" s="14"/>
       <c r="O77" s="2"/>
       <c r="Y77">
         <f t="shared" ref="Y77:Y102" si="1">P77+Q77+(U77*V77)+W77+X77+Z77</f>
@@ -4466,20 +4475,20 @@
       </c>
     </row>
     <row r="78" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="30"/>
-      <c r="B78" s="30"/>
-      <c r="C78" s="31"/>
-      <c r="D78" s="31"/>
-      <c r="E78" s="31"/>
-      <c r="F78" s="31"/>
-      <c r="G78" s="31"/>
-      <c r="H78" s="14"/>
-      <c r="I78" s="15"/>
+      <c r="A78" s="11"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="14"/>
       <c r="J78" s="5"/>
       <c r="K78" s="5"/>
-      <c r="L78" s="14"/>
-      <c r="M78" s="22"/>
-      <c r="N78" s="15"/>
+      <c r="L78" s="13"/>
+      <c r="M78" s="15"/>
+      <c r="N78" s="14"/>
       <c r="O78" s="2"/>
       <c r="Y78">
         <f t="shared" si="1"/>
@@ -4490,20 +4499,20 @@
       </c>
     </row>
     <row r="79" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="30"/>
-      <c r="B79" s="30"/>
-      <c r="C79" s="31"/>
-      <c r="D79" s="31"/>
-      <c r="E79" s="31"/>
-      <c r="F79" s="31"/>
-      <c r="G79" s="31"/>
-      <c r="H79" s="14"/>
-      <c r="I79" s="15"/>
+      <c r="A79" s="11"/>
+      <c r="B79" s="11"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="14"/>
       <c r="J79" s="5"/>
       <c r="K79" s="5"/>
-      <c r="L79" s="14"/>
-      <c r="M79" s="22"/>
-      <c r="N79" s="15"/>
+      <c r="L79" s="13"/>
+      <c r="M79" s="15"/>
+      <c r="N79" s="14"/>
       <c r="O79" s="2"/>
       <c r="Y79">
         <f t="shared" si="1"/>
@@ -4514,20 +4523,20 @@
       </c>
     </row>
     <row r="80" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="30"/>
-      <c r="B80" s="30"/>
-      <c r="C80" s="31"/>
-      <c r="D80" s="31"/>
-      <c r="E80" s="31"/>
-      <c r="F80" s="31"/>
-      <c r="G80" s="31"/>
-      <c r="H80" s="14"/>
-      <c r="I80" s="15"/>
+      <c r="A80" s="11"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="14"/>
       <c r="J80" s="5"/>
       <c r="K80" s="5"/>
-      <c r="L80" s="14"/>
-      <c r="M80" s="22"/>
-      <c r="N80" s="15"/>
+      <c r="L80" s="13"/>
+      <c r="M80" s="15"/>
+      <c r="N80" s="14"/>
       <c r="O80" s="2"/>
       <c r="Y80">
         <f t="shared" si="1"/>
@@ -4538,20 +4547,20 @@
       </c>
     </row>
     <row r="81" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="30"/>
-      <c r="B81" s="30"/>
-      <c r="C81" s="31"/>
-      <c r="D81" s="31"/>
-      <c r="E81" s="31"/>
-      <c r="F81" s="31"/>
-      <c r="G81" s="31"/>
-      <c r="H81" s="14"/>
-      <c r="I81" s="15"/>
+      <c r="A81" s="11"/>
+      <c r="B81" s="11"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="14"/>
       <c r="J81" s="5"/>
       <c r="K81" s="5"/>
-      <c r="L81" s="14"/>
-      <c r="M81" s="22"/>
-      <c r="N81" s="15"/>
+      <c r="L81" s="13"/>
+      <c r="M81" s="15"/>
+      <c r="N81" s="14"/>
       <c r="O81" s="2"/>
       <c r="Y81">
         <f t="shared" si="1"/>
@@ -4562,20 +4571,20 @@
       </c>
     </row>
     <row r="82" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="30"/>
-      <c r="B82" s="30"/>
-      <c r="C82" s="31"/>
-      <c r="D82" s="31"/>
-      <c r="E82" s="31"/>
-      <c r="F82" s="31"/>
-      <c r="G82" s="31"/>
-      <c r="H82" s="14"/>
-      <c r="I82" s="15"/>
+      <c r="A82" s="11"/>
+      <c r="B82" s="11"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="14"/>
       <c r="J82" s="5"/>
       <c r="K82" s="5"/>
-      <c r="L82" s="14"/>
-      <c r="M82" s="22"/>
-      <c r="N82" s="15"/>
+      <c r="L82" s="13"/>
+      <c r="M82" s="15"/>
+      <c r="N82" s="14"/>
       <c r="O82" s="2"/>
       <c r="Y82">
         <f t="shared" si="1"/>
@@ -4586,20 +4595,20 @@
       </c>
     </row>
     <row r="83" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="30"/>
-      <c r="B83" s="30"/>
-      <c r="C83" s="31"/>
-      <c r="D83" s="31"/>
-      <c r="E83" s="31"/>
-      <c r="F83" s="31"/>
-      <c r="G83" s="31"/>
-      <c r="H83" s="14"/>
-      <c r="I83" s="15"/>
+      <c r="A83" s="11"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+      <c r="G83" s="12"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="14"/>
       <c r="J83" s="5"/>
       <c r="K83" s="5"/>
-      <c r="L83" s="14"/>
-      <c r="M83" s="22"/>
-      <c r="N83" s="15"/>
+      <c r="L83" s="13"/>
+      <c r="M83" s="15"/>
+      <c r="N83" s="14"/>
       <c r="O83" s="2"/>
       <c r="Y83">
         <f t="shared" si="1"/>
@@ -4610,20 +4619,20 @@
       </c>
     </row>
     <row r="84" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="30"/>
-      <c r="B84" s="30"/>
-      <c r="C84" s="31"/>
-      <c r="D84" s="31"/>
-      <c r="E84" s="31"/>
-      <c r="F84" s="31"/>
-      <c r="G84" s="31"/>
-      <c r="H84" s="14"/>
-      <c r="I84" s="15"/>
+      <c r="A84" s="11"/>
+      <c r="B84" s="11"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="14"/>
       <c r="J84" s="5"/>
       <c r="K84" s="5"/>
-      <c r="L84" s="14"/>
-      <c r="M84" s="22"/>
-      <c r="N84" s="15"/>
+      <c r="L84" s="13"/>
+      <c r="M84" s="15"/>
+      <c r="N84" s="14"/>
       <c r="O84" s="2"/>
       <c r="Y84">
         <f t="shared" si="1"/>
@@ -4634,20 +4643,20 @@
       </c>
     </row>
     <row r="85" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="30"/>
-      <c r="B85" s="30"/>
-      <c r="C85" s="31"/>
-      <c r="D85" s="31"/>
-      <c r="E85" s="31"/>
-      <c r="F85" s="31"/>
-      <c r="G85" s="31"/>
-      <c r="H85" s="14"/>
-      <c r="I85" s="15"/>
+      <c r="A85" s="11"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="14"/>
       <c r="J85" s="5"/>
       <c r="K85" s="5"/>
-      <c r="L85" s="14"/>
-      <c r="M85" s="22"/>
-      <c r="N85" s="15"/>
+      <c r="L85" s="13"/>
+      <c r="M85" s="15"/>
+      <c r="N85" s="14"/>
       <c r="O85" s="2"/>
       <c r="Y85">
         <f t="shared" si="1"/>
@@ -4658,20 +4667,20 @@
       </c>
     </row>
     <row r="86" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="30"/>
-      <c r="B86" s="30"/>
-      <c r="C86" s="31"/>
-      <c r="D86" s="31"/>
-      <c r="E86" s="31"/>
-      <c r="F86" s="31"/>
-      <c r="G86" s="31"/>
-      <c r="H86" s="14"/>
-      <c r="I86" s="15"/>
+      <c r="A86" s="11"/>
+      <c r="B86" s="11"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12"/>
+      <c r="G86" s="12"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="14"/>
       <c r="J86" s="5"/>
       <c r="K86" s="5"/>
-      <c r="L86" s="14"/>
-      <c r="M86" s="22"/>
-      <c r="N86" s="15"/>
+      <c r="L86" s="13"/>
+      <c r="M86" s="15"/>
+      <c r="N86" s="14"/>
       <c r="O86" s="2"/>
       <c r="Y86">
         <f t="shared" si="1"/>
@@ -4682,20 +4691,20 @@
       </c>
     </row>
     <row r="87" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="30"/>
-      <c r="B87" s="30"/>
-      <c r="C87" s="31"/>
-      <c r="D87" s="31"/>
-      <c r="E87" s="31"/>
-      <c r="F87" s="31"/>
-      <c r="G87" s="31"/>
-      <c r="H87" s="14"/>
-      <c r="I87" s="15"/>
+      <c r="A87" s="11"/>
+      <c r="B87" s="11"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
+      <c r="F87" s="12"/>
+      <c r="G87" s="12"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="14"/>
       <c r="J87" s="5"/>
       <c r="K87" s="5"/>
-      <c r="L87" s="14"/>
-      <c r="M87" s="22"/>
-      <c r="N87" s="15"/>
+      <c r="L87" s="13"/>
+      <c r="M87" s="15"/>
+      <c r="N87" s="14"/>
       <c r="O87" s="2"/>
       <c r="Y87">
         <f t="shared" si="1"/>
@@ -4706,20 +4715,20 @@
       </c>
     </row>
     <row r="88" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="30"/>
-      <c r="B88" s="30"/>
-      <c r="C88" s="31"/>
-      <c r="D88" s="31"/>
-      <c r="E88" s="31"/>
-      <c r="F88" s="31"/>
-      <c r="G88" s="31"/>
-      <c r="H88" s="14"/>
-      <c r="I88" s="15"/>
+      <c r="A88" s="11"/>
+      <c r="B88" s="11"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="12"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="14"/>
       <c r="J88" s="5"/>
       <c r="K88" s="5"/>
-      <c r="L88" s="14"/>
-      <c r="M88" s="22"/>
-      <c r="N88" s="15"/>
+      <c r="L88" s="13"/>
+      <c r="M88" s="15"/>
+      <c r="N88" s="14"/>
       <c r="O88" s="2"/>
       <c r="Y88">
         <f t="shared" si="1"/>
@@ -4730,20 +4739,20 @@
       </c>
     </row>
     <row r="89" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="30"/>
-      <c r="B89" s="30"/>
-      <c r="C89" s="31"/>
-      <c r="D89" s="31"/>
-      <c r="E89" s="31"/>
-      <c r="F89" s="31"/>
-      <c r="G89" s="31"/>
-      <c r="H89" s="14"/>
-      <c r="I89" s="15"/>
+      <c r="A89" s="11"/>
+      <c r="B89" s="11"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="12"/>
+      <c r="G89" s="12"/>
+      <c r="H89" s="13"/>
+      <c r="I89" s="14"/>
       <c r="J89" s="5"/>
       <c r="K89" s="5"/>
-      <c r="L89" s="14"/>
-      <c r="M89" s="22"/>
-      <c r="N89" s="15"/>
+      <c r="L89" s="13"/>
+      <c r="M89" s="15"/>
+      <c r="N89" s="14"/>
       <c r="O89" s="2"/>
       <c r="Y89">
         <f t="shared" si="1"/>
@@ -4754,20 +4763,20 @@
       </c>
     </row>
     <row r="90" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="30"/>
-      <c r="B90" s="30"/>
-      <c r="C90" s="31"/>
-      <c r="D90" s="31"/>
-      <c r="E90" s="31"/>
-      <c r="F90" s="31"/>
-      <c r="G90" s="31"/>
-      <c r="H90" s="14"/>
-      <c r="I90" s="15"/>
+      <c r="A90" s="11"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="13"/>
+      <c r="I90" s="14"/>
       <c r="J90" s="5"/>
       <c r="K90" s="5"/>
-      <c r="L90" s="14"/>
-      <c r="M90" s="22"/>
-      <c r="N90" s="15"/>
+      <c r="L90" s="13"/>
+      <c r="M90" s="15"/>
+      <c r="N90" s="14"/>
       <c r="O90" s="2"/>
       <c r="Y90">
         <f t="shared" si="1"/>
@@ -4778,20 +4787,20 @@
       </c>
     </row>
     <row r="91" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="30"/>
-      <c r="B91" s="30"/>
-      <c r="C91" s="31"/>
-      <c r="D91" s="31"/>
-      <c r="E91" s="31"/>
-      <c r="F91" s="31"/>
-      <c r="G91" s="31"/>
-      <c r="H91" s="14"/>
-      <c r="I91" s="15"/>
+      <c r="A91" s="11"/>
+      <c r="B91" s="11"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="13"/>
+      <c r="I91" s="14"/>
       <c r="J91" s="5"/>
       <c r="K91" s="5"/>
-      <c r="L91" s="14"/>
-      <c r="M91" s="22"/>
-      <c r="N91" s="15"/>
+      <c r="L91" s="13"/>
+      <c r="M91" s="15"/>
+      <c r="N91" s="14"/>
       <c r="O91" s="2"/>
       <c r="Y91">
         <f t="shared" si="1"/>
@@ -4802,20 +4811,20 @@
       </c>
     </row>
     <row r="92" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="30"/>
-      <c r="B92" s="30"/>
-      <c r="C92" s="31"/>
-      <c r="D92" s="31"/>
-      <c r="E92" s="31"/>
-      <c r="F92" s="31"/>
-      <c r="G92" s="31"/>
-      <c r="H92" s="14"/>
-      <c r="I92" s="15"/>
+      <c r="A92" s="11"/>
+      <c r="B92" s="11"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="14"/>
       <c r="J92" s="5"/>
       <c r="K92" s="5"/>
-      <c r="L92" s="14"/>
-      <c r="M92" s="22"/>
-      <c r="N92" s="15"/>
+      <c r="L92" s="13"/>
+      <c r="M92" s="15"/>
+      <c r="N92" s="14"/>
       <c r="O92" s="2"/>
       <c r="Y92">
         <f t="shared" si="1"/>
@@ -4826,20 +4835,20 @@
       </c>
     </row>
     <row r="93" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="30"/>
-      <c r="B93" s="30"/>
-      <c r="C93" s="31"/>
-      <c r="D93" s="31"/>
-      <c r="E93" s="31"/>
-      <c r="F93" s="31"/>
-      <c r="G93" s="31"/>
-      <c r="H93" s="14"/>
-      <c r="I93" s="15"/>
+      <c r="A93" s="11"/>
+      <c r="B93" s="11"/>
+      <c r="C93" s="12"/>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
+      <c r="F93" s="12"/>
+      <c r="G93" s="12"/>
+      <c r="H93" s="13"/>
+      <c r="I93" s="14"/>
       <c r="J93" s="5"/>
       <c r="K93" s="5"/>
-      <c r="L93" s="14"/>
-      <c r="M93" s="22"/>
-      <c r="N93" s="15"/>
+      <c r="L93" s="13"/>
+      <c r="M93" s="15"/>
+      <c r="N93" s="14"/>
       <c r="O93" s="2"/>
       <c r="Y93">
         <f t="shared" si="1"/>
@@ -4850,20 +4859,20 @@
       </c>
     </row>
     <row r="94" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="30"/>
-      <c r="B94" s="30"/>
-      <c r="C94" s="31"/>
-      <c r="D94" s="31"/>
-      <c r="E94" s="31"/>
-      <c r="F94" s="31"/>
-      <c r="G94" s="31"/>
-      <c r="H94" s="14"/>
-      <c r="I94" s="15"/>
+      <c r="A94" s="11"/>
+      <c r="B94" s="11"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="12"/>
+      <c r="H94" s="13"/>
+      <c r="I94" s="14"/>
       <c r="J94" s="5"/>
       <c r="K94" s="5"/>
-      <c r="L94" s="14"/>
-      <c r="M94" s="22"/>
-      <c r="N94" s="15"/>
+      <c r="L94" s="13"/>
+      <c r="M94" s="15"/>
+      <c r="N94" s="14"/>
       <c r="O94" s="2"/>
       <c r="Y94">
         <f t="shared" si="1"/>
@@ -4874,20 +4883,20 @@
       </c>
     </row>
     <row r="95" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="30"/>
-      <c r="B95" s="30"/>
-      <c r="C95" s="31"/>
-      <c r="D95" s="31"/>
-      <c r="E95" s="31"/>
-      <c r="F95" s="31"/>
-      <c r="G95" s="31"/>
-      <c r="H95" s="14"/>
-      <c r="I95" s="15"/>
+      <c r="A95" s="11"/>
+      <c r="B95" s="11"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="12"/>
+      <c r="H95" s="13"/>
+      <c r="I95" s="14"/>
       <c r="J95" s="5"/>
       <c r="K95" s="5"/>
-      <c r="L95" s="14"/>
-      <c r="M95" s="22"/>
-      <c r="N95" s="15"/>
+      <c r="L95" s="13"/>
+      <c r="M95" s="15"/>
+      <c r="N95" s="14"/>
       <c r="O95" s="2"/>
       <c r="Y95">
         <f t="shared" si="1"/>
@@ -4898,20 +4907,20 @@
       </c>
     </row>
     <row r="96" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="30"/>
-      <c r="B96" s="30"/>
-      <c r="C96" s="31"/>
-      <c r="D96" s="31"/>
-      <c r="E96" s="31"/>
-      <c r="F96" s="31"/>
-      <c r="G96" s="31"/>
-      <c r="H96" s="14"/>
-      <c r="I96" s="15"/>
+      <c r="A96" s="11"/>
+      <c r="B96" s="11"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12"/>
+      <c r="F96" s="12"/>
+      <c r="G96" s="12"/>
+      <c r="H96" s="13"/>
+      <c r="I96" s="14"/>
       <c r="J96" s="5"/>
       <c r="K96" s="5"/>
-      <c r="L96" s="14"/>
-      <c r="M96" s="22"/>
-      <c r="N96" s="15"/>
+      <c r="L96" s="13"/>
+      <c r="M96" s="15"/>
+      <c r="N96" s="14"/>
       <c r="O96" s="2"/>
       <c r="Y96">
         <f t="shared" si="1"/>
@@ -4922,20 +4931,20 @@
       </c>
     </row>
     <row r="97" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="30"/>
-      <c r="B97" s="30"/>
-      <c r="C97" s="31"/>
-      <c r="D97" s="31"/>
-      <c r="E97" s="31"/>
-      <c r="F97" s="31"/>
-      <c r="G97" s="31"/>
-      <c r="H97" s="14"/>
-      <c r="I97" s="15"/>
+      <c r="A97" s="11"/>
+      <c r="B97" s="11"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="13"/>
+      <c r="I97" s="14"/>
       <c r="J97" s="5"/>
       <c r="K97" s="5"/>
-      <c r="L97" s="14"/>
-      <c r="M97" s="22"/>
-      <c r="N97" s="15"/>
+      <c r="L97" s="13"/>
+      <c r="M97" s="15"/>
+      <c r="N97" s="14"/>
       <c r="O97" s="2"/>
       <c r="Y97">
         <f t="shared" si="1"/>
@@ -4946,20 +4955,20 @@
       </c>
     </row>
     <row r="98" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="30"/>
-      <c r="B98" s="30"/>
-      <c r="C98" s="31"/>
-      <c r="D98" s="31"/>
-      <c r="E98" s="31"/>
-      <c r="F98" s="31"/>
-      <c r="G98" s="31"/>
-      <c r="H98" s="14"/>
-      <c r="I98" s="15"/>
+      <c r="A98" s="11"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="13"/>
+      <c r="I98" s="14"/>
       <c r="J98" s="5"/>
       <c r="K98" s="5"/>
-      <c r="L98" s="14"/>
-      <c r="M98" s="22"/>
-      <c r="N98" s="15"/>
+      <c r="L98" s="13"/>
+      <c r="M98" s="15"/>
+      <c r="N98" s="14"/>
       <c r="O98" s="2"/>
       <c r="Y98">
         <f t="shared" si="1"/>
@@ -4970,20 +4979,20 @@
       </c>
     </row>
     <row r="99" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="30"/>
-      <c r="B99" s="30"/>
-      <c r="C99" s="31"/>
-      <c r="D99" s="31"/>
-      <c r="E99" s="31"/>
-      <c r="F99" s="31"/>
-      <c r="G99" s="31"/>
-      <c r="H99" s="14"/>
-      <c r="I99" s="15"/>
+      <c r="A99" s="11"/>
+      <c r="B99" s="11"/>
+      <c r="C99" s="12"/>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="12"/>
+      <c r="H99" s="13"/>
+      <c r="I99" s="14"/>
       <c r="J99" s="5"/>
       <c r="K99" s="5"/>
-      <c r="L99" s="14"/>
-      <c r="M99" s="22"/>
-      <c r="N99" s="15"/>
+      <c r="L99" s="13"/>
+      <c r="M99" s="15"/>
+      <c r="N99" s="14"/>
       <c r="O99" s="2"/>
       <c r="Y99">
         <f t="shared" si="1"/>
@@ -4994,20 +5003,20 @@
       </c>
     </row>
     <row r="100" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="30"/>
-      <c r="B100" s="30"/>
-      <c r="C100" s="31"/>
-      <c r="D100" s="31"/>
-      <c r="E100" s="31"/>
-      <c r="F100" s="31"/>
-      <c r="G100" s="31"/>
-      <c r="H100" s="14"/>
-      <c r="I100" s="15"/>
+      <c r="A100" s="11"/>
+      <c r="B100" s="11"/>
+      <c r="C100" s="12"/>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="12"/>
+      <c r="H100" s="13"/>
+      <c r="I100" s="14"/>
       <c r="J100" s="5"/>
       <c r="K100" s="5"/>
-      <c r="L100" s="14"/>
-      <c r="M100" s="22"/>
-      <c r="N100" s="15"/>
+      <c r="L100" s="13"/>
+      <c r="M100" s="15"/>
+      <c r="N100" s="14"/>
       <c r="O100" s="2"/>
       <c r="Y100">
         <f t="shared" si="1"/>
@@ -5018,20 +5027,20 @@
       </c>
     </row>
     <row r="101" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="30"/>
-      <c r="B101" s="30"/>
-      <c r="C101" s="31"/>
-      <c r="D101" s="31"/>
-      <c r="E101" s="31"/>
-      <c r="F101" s="31"/>
-      <c r="G101" s="31"/>
-      <c r="H101" s="14"/>
-      <c r="I101" s="15"/>
+      <c r="A101" s="11"/>
+      <c r="B101" s="11"/>
+      <c r="C101" s="12"/>
+      <c r="D101" s="12"/>
+      <c r="E101" s="12"/>
+      <c r="F101" s="12"/>
+      <c r="G101" s="12"/>
+      <c r="H101" s="13"/>
+      <c r="I101" s="14"/>
       <c r="J101" s="5"/>
       <c r="K101" s="5"/>
-      <c r="L101" s="14"/>
-      <c r="M101" s="22"/>
-      <c r="N101" s="15"/>
+      <c r="L101" s="13"/>
+      <c r="M101" s="15"/>
+      <c r="N101" s="14"/>
       <c r="O101" s="2"/>
       <c r="Y101">
         <f t="shared" si="1"/>
@@ -5042,20 +5051,20 @@
       </c>
     </row>
     <row r="102" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="30"/>
-      <c r="B102" s="30"/>
-      <c r="C102" s="31"/>
-      <c r="D102" s="31"/>
-      <c r="E102" s="31"/>
-      <c r="F102" s="31"/>
-      <c r="G102" s="31"/>
-      <c r="H102" s="14"/>
-      <c r="I102" s="15"/>
+      <c r="A102" s="11"/>
+      <c r="B102" s="11"/>
+      <c r="C102" s="12"/>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
+      <c r="F102" s="12"/>
+      <c r="G102" s="12"/>
+      <c r="H102" s="13"/>
+      <c r="I102" s="14"/>
       <c r="J102" s="5"/>
       <c r="K102" s="5"/>
-      <c r="L102" s="14"/>
-      <c r="M102" s="22"/>
-      <c r="N102" s="15"/>
+      <c r="L102" s="13"/>
+      <c r="M102" s="15"/>
+      <c r="N102" s="14"/>
       <c r="O102" s="2"/>
       <c r="Y102">
         <f t="shared" si="1"/>
@@ -5076,6 +5085,464 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="482">
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:M4"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="L21:N21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="L26:N26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="L28:N28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="L29:N29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="L30:N30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="L32:N32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="L33:N33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="L35:N35"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="L39:N39"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="L36:N36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="L37:N37"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="L43:N43"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="L38:N38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="L41:N41"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="L44:N44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="L45:N45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="L46:N46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="L47:N47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="L48:N48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="L49:N49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="L50:N50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="L51:N51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="L52:N52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="L53:N53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="L54:N54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="L55:N55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="L56:N56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="L57:N57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="L58:N58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="L59:N59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="L60:N60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="L61:N61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="L62:N62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="L63:N63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="L64:N64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="L65:N65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="L66:N66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="L67:N67"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="L72:N72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="L73:N73"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="L70:N70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="L71:N71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="L68:N68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="L69:N69"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="L77:N77"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="E75:G75"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="L75:N75"/>
+    <mergeCell ref="L74:N74"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="E78:G78"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="L78:N78"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="L76:N76"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="H79:I79"/>
+    <mergeCell ref="L79:N79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="L80:N80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="E81:G81"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="L81:N81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="E82:G82"/>
+    <mergeCell ref="H82:I82"/>
+    <mergeCell ref="L82:N82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="E83:G83"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="L83:N83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="E84:G84"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="L84:N84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="E85:G85"/>
+    <mergeCell ref="H85:I85"/>
+    <mergeCell ref="L85:N85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="E86:G86"/>
+    <mergeCell ref="H86:I86"/>
+    <mergeCell ref="L86:N86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="E87:G87"/>
+    <mergeCell ref="H87:I87"/>
+    <mergeCell ref="L87:N87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="E88:G88"/>
+    <mergeCell ref="H88:I88"/>
+    <mergeCell ref="L88:N88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="E89:G89"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="L89:N89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="E90:G90"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="L90:N90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="E91:G91"/>
+    <mergeCell ref="H91:I91"/>
+    <mergeCell ref="L91:N91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="E92:G92"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="L92:N92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="E93:G93"/>
+    <mergeCell ref="H93:I93"/>
+    <mergeCell ref="L93:N93"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="E97:G97"/>
+    <mergeCell ref="H97:I97"/>
+    <mergeCell ref="L97:N97"/>
+    <mergeCell ref="L101:N101"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="E94:G94"/>
+    <mergeCell ref="H94:I94"/>
+    <mergeCell ref="L94:N94"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="E99:G99"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="L99:N99"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="E95:G95"/>
+    <mergeCell ref="H95:I95"/>
+    <mergeCell ref="L95:N95"/>
     <mergeCell ref="A102:B102"/>
     <mergeCell ref="C102:D102"/>
     <mergeCell ref="E102:G102"/>
@@ -5100,464 +5567,6 @@
     <mergeCell ref="C101:D101"/>
     <mergeCell ref="E101:G101"/>
     <mergeCell ref="H101:I101"/>
-    <mergeCell ref="L101:N101"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="E94:G94"/>
-    <mergeCell ref="H94:I94"/>
-    <mergeCell ref="L94:N94"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="E99:G99"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="L99:N99"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="E95:G95"/>
-    <mergeCell ref="H95:I95"/>
-    <mergeCell ref="L95:N95"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="E93:G93"/>
-    <mergeCell ref="H93:I93"/>
-    <mergeCell ref="L93:N93"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="E97:G97"/>
-    <mergeCell ref="H97:I97"/>
-    <mergeCell ref="L97:N97"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="E91:G91"/>
-    <mergeCell ref="H91:I91"/>
-    <mergeCell ref="L91:N91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="E92:G92"/>
-    <mergeCell ref="H92:I92"/>
-    <mergeCell ref="L92:N92"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="E89:G89"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="L89:N89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="E90:G90"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="L90:N90"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="E87:G87"/>
-    <mergeCell ref="H87:I87"/>
-    <mergeCell ref="L87:N87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="E88:G88"/>
-    <mergeCell ref="H88:I88"/>
-    <mergeCell ref="L88:N88"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="E85:G85"/>
-    <mergeCell ref="H85:I85"/>
-    <mergeCell ref="L85:N85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="E86:G86"/>
-    <mergeCell ref="H86:I86"/>
-    <mergeCell ref="L86:N86"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="E83:G83"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="L83:N83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="E84:G84"/>
-    <mergeCell ref="H84:I84"/>
-    <mergeCell ref="L84:N84"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="E81:G81"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="L81:N81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="E82:G82"/>
-    <mergeCell ref="H82:I82"/>
-    <mergeCell ref="L82:N82"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="E79:G79"/>
-    <mergeCell ref="H79:I79"/>
-    <mergeCell ref="L79:N79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="H80:I80"/>
-    <mergeCell ref="L80:N80"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="E78:G78"/>
-    <mergeCell ref="H78:I78"/>
-    <mergeCell ref="L78:N78"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="L76:N76"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="E77:G77"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="L77:N77"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="L75:N75"/>
-    <mergeCell ref="L74:N74"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="L68:N68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="L69:N69"/>
-    <mergeCell ref="E72:G72"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="L72:N72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="H73:I73"/>
-    <mergeCell ref="L73:N73"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="L70:N70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="L71:N71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="L66:N66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="L67:N67"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="L64:N64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="L65:N65"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="L62:N62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="L63:N63"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="L60:N60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="L61:N61"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="L58:N58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="L59:N59"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="L56:N56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="L57:N57"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="L54:N54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="L55:N55"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="L52:N52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="L53:N53"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="L50:N50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="L51:N51"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="L48:N48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="L49:N49"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="L46:N46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="L47:N47"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="L44:N44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="L45:N45"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="L43:N43"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="L38:N38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="L41:N41"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="L39:N39"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="L36:N36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="L37:N37"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="L35:N35"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="L32:N32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="L33:N33"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="L28:N28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="L29:N29"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="L26:N26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="L24:N24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="L25:N25"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="L23:N23"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="L20:N20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="L21:N21"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:M4"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="I7:M7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <pageMargins left="0.39" right="0.39" top="0.39" bottom="0.39" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>